<commit_message>
Updated excel calcs to match shiny tool
</commit_message>
<xml_diff>
--- a/eSurvey_Expected_Completes_Calculator/ExpectedCompletesExcelTool.xlsx
+++ b/eSurvey_Expected_Completes_Calculator/ExpectedCompletesExcelTool.xlsx
@@ -379,16 +379,19 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -397,11 +400,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,7 +686,7 @@
   <dimension ref="A1:V181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,17 +708,17 @@
   <sheetData>
     <row r="1" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="21">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F1" s="21">
+      <c r="E1" s="17">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F1" s="17">
         <v>0.61</v>
       </c>
       <c r="G1" s="1"/>
@@ -740,16 +740,16 @@
     </row>
     <row r="2" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="22" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="21">
-        <v>0.59</v>
-      </c>
-      <c r="F2" s="21">
-        <v>0.55000000000000004</v>
+      <c r="E2" s="17">
+        <v>0.19</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.72</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -770,16 +770,16 @@
     </row>
     <row r="3" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="22" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="21">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="F3" s="21">
-        <v>0.72</v>
+      <c r="E3" s="17">
+        <v>0.27</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0.55000000000000004</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -817,7 +817,7 @@
       <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="15" t="s">
         <v>28</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -870,30 +870,30 @@
         <v>10000</v>
       </c>
       <c r="E5" s="10">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F5" s="11">
         <v>0.61</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="16">
         <f>IF(ISBLANK(B5),"--",SUM(H5,I5))</f>
-        <v>596</v>
+        <v>821</v>
       </c>
       <c r="H5" s="8">
-        <f>IF(ISBLANK(B5),"--",ROUND(P5*INDEX(Lists!$F$2:$H$5,MATCH(B5,Lists!$F$2:$F$5,0),MATCH(C5,Lists!$F$2:$H$2,0)),0))</f>
-        <v>403</v>
+        <f>IF(ISBLANK(B5),"--",ROUND(P5*INDEX(Lists!$G$3:$G$5,MATCH(B5,Lists!$F$3:$F$5,0)),0))</f>
+        <v>612</v>
       </c>
       <c r="I5" s="7">
-        <f>IF($C5="eSurvey+SMS",ROUND(Q5*INDEX(Lists!$F$2:$H$5,MATCH(B5,Lists!$F$2:$F$5,0),MATCH(C5,Lists!$F$2:$H$2,0)),0),"--")</f>
-        <v>193</v>
+        <f>IF($C5="eSurvey+SMS",ROUND(Q5*INDEX(Lists!$H$3:$H$5,MATCH(B5,Lists!$F$3:$F$5,0)),0),"--")</f>
+        <v>209</v>
       </c>
       <c r="J5" s="8">
         <f>IF(ISBLANK(B5),"--",P5-H5)</f>
-        <v>2285</v>
+        <v>2172</v>
       </c>
       <c r="K5" s="8">
         <f>IF($C5="eSurvey+SMS",Q5-I5,"--")</f>
-        <v>1095</v>
+        <v>1021</v>
       </c>
       <c r="L5" s="12">
         <f>IF(ISBLANK(B5),"--",N5)</f>
@@ -901,7 +901,7 @@
       </c>
       <c r="M5" s="12">
         <f>IF(ISBLANK(B5),"--",O5-SUM(P5,Q5))</f>
-        <v>824</v>
+        <v>786</v>
       </c>
       <c r="N5" s="1">
         <f>IF(ISNA(ROUND(D5*INDEX(Lists!$J$2:$L$5,MATCH(B5,Lists!$J$2:$J$5,0),MATCH(C5,Lists!$J$2:$L$2,0)),0)),0,ROUND(D5*INDEX(Lists!$J$2:$L$5,MATCH(B5,Lists!$J$2:$J$5,0),MATCH(C5,Lists!$J$2:$L$2,0)),0))</f>
@@ -913,11 +913,11 @@
       </c>
       <c r="P5" s="1">
         <f>ROUND(O5*E5,0)</f>
-        <v>2688</v>
+        <v>2784</v>
       </c>
       <c r="Q5" s="1">
         <f>ROUND(((O5-P5)*F5),0)</f>
-        <v>1288</v>
+        <v>1230</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -932,16 +932,16 @@
       <c r="D6" s="12"/>
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="18" t="str">
+      <c r="G6" s="16" t="str">
         <f t="shared" ref="G6:G69" si="0">IF(ISBLANK(B6),"--",SUM(H6,I6))</f>
         <v>--</v>
       </c>
       <c r="H6" s="8" t="str">
-        <f>IF(ISBLANK(B6),"--",ROUND(P6*INDEX(Lists!$F$2:$H$5,MATCH(B6,Lists!$F$2:$F$5,0),MATCH(C6,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B6),"--",ROUND(P6*INDEX(Lists!$G$3:$G$5,MATCH(B6,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I6" s="7" t="str">
-        <f>IF($C6="eSurvey+SMS",ROUND(Q6*INDEX(Lists!$F$2:$H$5,MATCH(B6,Lists!$F$2:$F$5,0),MATCH(C6,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C6="eSurvey+SMS",ROUND(Q6*INDEX(Lists!$H$3:$H$5,MATCH(B6,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J6" s="8" t="str">
@@ -989,16 +989,16 @@
       <c r="D7" s="12"/>
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="18" t="str">
+      <c r="G7" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H7" s="8" t="str">
-        <f>IF(ISBLANK(B7),"--",ROUND(P7*INDEX(Lists!$F$2:$H$5,MATCH(B7,Lists!$F$2:$F$5,0),MATCH(C7,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B7),"--",ROUND(P7*INDEX(Lists!$G$3:$G$5,MATCH(B7,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I7" s="7" t="str">
-        <f>IF($C7="eSurvey+SMS",ROUND(Q7*INDEX(Lists!$F$2:$H$5,MATCH(B7,Lists!$F$2:$F$5,0),MATCH(C7,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C7="eSurvey+SMS",ROUND(Q7*INDEX(Lists!$H$3:$H$5,MATCH(B7,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J7" s="8" t="str">
@@ -1046,16 +1046,16 @@
       <c r="D8" s="12"/>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="18" t="str">
+      <c r="G8" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H8" s="8" t="str">
-        <f>IF(ISBLANK(B8),"--",ROUND(P8*INDEX(Lists!$F$2:$H$5,MATCH(B8,Lists!$F$2:$F$5,0),MATCH(C8,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B8),"--",ROUND(P8*INDEX(Lists!$G$3:$G$5,MATCH(B8,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I8" s="7" t="str">
-        <f>IF($C8="eSurvey+SMS",ROUND(Q8*INDEX(Lists!$F$2:$H$5,MATCH(B8,Lists!$F$2:$F$5,0),MATCH(C8,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C8="eSurvey+SMS",ROUND(Q8*INDEX(Lists!$H$3:$H$5,MATCH(B8,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J8" s="8" t="str">
@@ -1103,16 +1103,16 @@
       <c r="D9" s="12"/>
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="18" t="str">
+      <c r="G9" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H9" s="8" t="str">
-        <f>IF(ISBLANK(B9),"--",ROUND(P9*INDEX(Lists!$F$2:$H$5,MATCH(B9,Lists!$F$2:$F$5,0),MATCH(C9,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B9),"--",ROUND(P9*INDEX(Lists!$G$3:$G$5,MATCH(B9,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I9" s="7" t="str">
-        <f>IF($C9="eSurvey+SMS",ROUND(Q9*INDEX(Lists!$F$2:$H$5,MATCH(B9,Lists!$F$2:$F$5,0),MATCH(C9,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C9="eSurvey+SMS",ROUND(Q9*INDEX(Lists!$H$3:$H$5,MATCH(B9,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J9" s="8" t="str">
@@ -1160,16 +1160,16 @@
       <c r="D10" s="12"/>
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="18" t="str">
+      <c r="G10" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H10" s="8" t="str">
-        <f>IF(ISBLANK(B10),"--",ROUND(P10*INDEX(Lists!$F$2:$H$5,MATCH(B10,Lists!$F$2:$F$5,0),MATCH(C10,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B10),"--",ROUND(P10*INDEX(Lists!$G$3:$G$5,MATCH(B10,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I10" s="7" t="str">
-        <f>IF($C10="eSurvey+SMS",ROUND(Q10*INDEX(Lists!$F$2:$H$5,MATCH(B10,Lists!$F$2:$F$5,0),MATCH(C10,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C10="eSurvey+SMS",ROUND(Q10*INDEX(Lists!$H$3:$H$5,MATCH(B10,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J10" s="8" t="str">
@@ -1217,16 +1217,16 @@
       <c r="D11" s="12"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="18" t="str">
+      <c r="G11" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H11" s="8" t="str">
-        <f>IF(ISBLANK(B11),"--",ROUND(P11*INDEX(Lists!$F$2:$H$5,MATCH(B11,Lists!$F$2:$F$5,0),MATCH(C11,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B11),"--",ROUND(P11*INDEX(Lists!$G$3:$G$5,MATCH(B11,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I11" s="7" t="str">
-        <f>IF($C11="eSurvey+SMS",ROUND(Q11*INDEX(Lists!$F$2:$H$5,MATCH(B11,Lists!$F$2:$F$5,0),MATCH(C11,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C11="eSurvey+SMS",ROUND(Q11*INDEX(Lists!$H$3:$H$5,MATCH(B11,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J11" s="8" t="str">
@@ -1274,16 +1274,16 @@
       <c r="D12" s="12"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="18" t="str">
+      <c r="G12" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H12" s="8" t="str">
-        <f>IF(ISBLANK(B12),"--",ROUND(P12*INDEX(Lists!$F$2:$H$5,MATCH(B12,Lists!$F$2:$F$5,0),MATCH(C12,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B12),"--",ROUND(P12*INDEX(Lists!$G$3:$G$5,MATCH(B12,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I12" s="7" t="str">
-        <f>IF($C12="eSurvey+SMS",ROUND(Q12*INDEX(Lists!$F$2:$H$5,MATCH(B12,Lists!$F$2:$F$5,0),MATCH(C12,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C12="eSurvey+SMS",ROUND(Q12*INDEX(Lists!$H$3:$H$5,MATCH(B12,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J12" s="8" t="str">
@@ -1331,16 +1331,16 @@
       <c r="D13" s="12"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="18" t="str">
+      <c r="G13" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H13" s="8" t="str">
-        <f>IF(ISBLANK(B13),"--",ROUND(P13*INDEX(Lists!$F$2:$H$5,MATCH(B13,Lists!$F$2:$F$5,0),MATCH(C13,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B13),"--",ROUND(P13*INDEX(Lists!$G$3:$G$5,MATCH(B13,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I13" s="7" t="str">
-        <f>IF($C13="eSurvey+SMS",ROUND(Q13*INDEX(Lists!$F$2:$H$5,MATCH(B13,Lists!$F$2:$F$5,0),MATCH(C13,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C13="eSurvey+SMS",ROUND(Q13*INDEX(Lists!$H$3:$H$5,MATCH(B13,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J13" s="8" t="str">
@@ -1388,16 +1388,16 @@
       <c r="D14" s="12"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
-      <c r="G14" s="18" t="str">
+      <c r="G14" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H14" s="8" t="str">
-        <f>IF(ISBLANK(B14),"--",ROUND(P14*INDEX(Lists!$F$2:$H$5,MATCH(B14,Lists!$F$2:$F$5,0),MATCH(C14,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B14),"--",ROUND(P14*INDEX(Lists!$G$3:$G$5,MATCH(B14,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I14" s="7" t="str">
-        <f>IF($C14="eSurvey+SMS",ROUND(Q14*INDEX(Lists!$F$2:$H$5,MATCH(B14,Lists!$F$2:$F$5,0),MATCH(C14,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C14="eSurvey+SMS",ROUND(Q14*INDEX(Lists!$H$3:$H$5,MATCH(B14,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J14" s="8" t="str">
@@ -1445,16 +1445,16 @@
       <c r="D15" s="12"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="18" t="str">
+      <c r="G15" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H15" s="8" t="str">
-        <f>IF(ISBLANK(B15),"--",ROUND(P15*INDEX(Lists!$F$2:$H$5,MATCH(B15,Lists!$F$2:$F$5,0),MATCH(C15,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B15),"--",ROUND(P15*INDEX(Lists!$G$3:$G$5,MATCH(B15,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I15" s="7" t="str">
-        <f>IF($C15="eSurvey+SMS",ROUND(Q15*INDEX(Lists!$F$2:$H$5,MATCH(B15,Lists!$F$2:$F$5,0),MATCH(C15,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C15="eSurvey+SMS",ROUND(Q15*INDEX(Lists!$H$3:$H$5,MATCH(B15,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J15" s="8" t="str">
@@ -1502,16 +1502,16 @@
       <c r="D16" s="12"/>
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="18" t="str">
+      <c r="G16" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H16" s="8" t="str">
-        <f>IF(ISBLANK(B16),"--",ROUND(P16*INDEX(Lists!$F$2:$H$5,MATCH(B16,Lists!$F$2:$F$5,0),MATCH(C16,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B16),"--",ROUND(P16*INDEX(Lists!$G$3:$G$5,MATCH(B16,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I16" s="7" t="str">
-        <f>IF($C16="eSurvey+SMS",ROUND(Q16*INDEX(Lists!$F$2:$H$5,MATCH(B16,Lists!$F$2:$F$5,0),MATCH(C16,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C16="eSurvey+SMS",ROUND(Q16*INDEX(Lists!$H$3:$H$5,MATCH(B16,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J16" s="8" t="str">
@@ -1559,16 +1559,16 @@
       <c r="D17" s="12"/>
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="18" t="str">
+      <c r="G17" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H17" s="8" t="str">
-        <f>IF(ISBLANK(B17),"--",ROUND(P17*INDEX(Lists!$F$2:$H$5,MATCH(B17,Lists!$F$2:$F$5,0),MATCH(C17,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B17),"--",ROUND(P17*INDEX(Lists!$G$3:$G$5,MATCH(B17,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I17" s="7" t="str">
-        <f>IF($C17="eSurvey+SMS",ROUND(Q17*INDEX(Lists!$F$2:$H$5,MATCH(B17,Lists!$F$2:$F$5,0),MATCH(C17,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C17="eSurvey+SMS",ROUND(Q17*INDEX(Lists!$H$3:$H$5,MATCH(B17,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J17" s="8" t="str">
@@ -1616,16 +1616,16 @@
       <c r="D18" s="12"/>
       <c r="E18" s="10"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="18" t="str">
+      <c r="G18" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H18" s="8" t="str">
-        <f>IF(ISBLANK(B18),"--",ROUND(P18*INDEX(Lists!$F$2:$H$5,MATCH(B18,Lists!$F$2:$F$5,0),MATCH(C18,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B18),"--",ROUND(P18*INDEX(Lists!$G$3:$G$5,MATCH(B18,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I18" s="7" t="str">
-        <f>IF($C18="eSurvey+SMS",ROUND(Q18*INDEX(Lists!$F$2:$H$5,MATCH(B18,Lists!$F$2:$F$5,0),MATCH(C18,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C18="eSurvey+SMS",ROUND(Q18*INDEX(Lists!$H$3:$H$5,MATCH(B18,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J18" s="8" t="str">
@@ -1673,16 +1673,16 @@
       <c r="D19" s="12"/>
       <c r="E19" s="10"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="18" t="str">
+      <c r="G19" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H19" s="8" t="str">
-        <f>IF(ISBLANK(B19),"--",ROUND(P19*INDEX(Lists!$F$2:$H$5,MATCH(B19,Lists!$F$2:$F$5,0),MATCH(C19,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B19),"--",ROUND(P19*INDEX(Lists!$G$3:$G$5,MATCH(B19,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I19" s="7" t="str">
-        <f>IF($C19="eSurvey+SMS",ROUND(Q19*INDEX(Lists!$F$2:$H$5,MATCH(B19,Lists!$F$2:$F$5,0),MATCH(C19,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C19="eSurvey+SMS",ROUND(Q19*INDEX(Lists!$H$3:$H$5,MATCH(B19,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J19" s="8" t="str">
@@ -1730,16 +1730,16 @@
       <c r="D20" s="12"/>
       <c r="E20" s="10"/>
       <c r="F20" s="11"/>
-      <c r="G20" s="18" t="str">
+      <c r="G20" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H20" s="8" t="str">
-        <f>IF(ISBLANK(B20),"--",ROUND(P20*INDEX(Lists!$F$2:$H$5,MATCH(B20,Lists!$F$2:$F$5,0),MATCH(C20,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B20),"--",ROUND(P20*INDEX(Lists!$G$3:$G$5,MATCH(B20,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I20" s="7" t="str">
-        <f>IF($C20="eSurvey+SMS",ROUND(Q20*INDEX(Lists!$F$2:$H$5,MATCH(B20,Lists!$F$2:$F$5,0),MATCH(C20,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C20="eSurvey+SMS",ROUND(Q20*INDEX(Lists!$H$3:$H$5,MATCH(B20,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J20" s="8" t="str">
@@ -1787,16 +1787,16 @@
       <c r="D21" s="12"/>
       <c r="E21" s="10"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="18" t="str">
+      <c r="G21" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H21" s="8" t="str">
-        <f>IF(ISBLANK(B21),"--",ROUND(P21*INDEX(Lists!$F$2:$H$5,MATCH(B21,Lists!$F$2:$F$5,0),MATCH(C21,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B21),"--",ROUND(P21*INDEX(Lists!$G$3:$G$5,MATCH(B21,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I21" s="7" t="str">
-        <f>IF($C21="eSurvey+SMS",ROUND(Q21*INDEX(Lists!$F$2:$H$5,MATCH(B21,Lists!$F$2:$F$5,0),MATCH(C21,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C21="eSurvey+SMS",ROUND(Q21*INDEX(Lists!$H$3:$H$5,MATCH(B21,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J21" s="8" t="str">
@@ -1844,16 +1844,16 @@
       <c r="D22" s="12"/>
       <c r="E22" s="10"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="18" t="str">
+      <c r="G22" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H22" s="8" t="str">
-        <f>IF(ISBLANK(B22),"--",ROUND(P22*INDEX(Lists!$F$2:$H$5,MATCH(B22,Lists!$F$2:$F$5,0),MATCH(C22,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B22),"--",ROUND(P22*INDEX(Lists!$G$3:$G$5,MATCH(B22,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I22" s="7" t="str">
-        <f>IF($C22="eSurvey+SMS",ROUND(Q22*INDEX(Lists!$F$2:$H$5,MATCH(B22,Lists!$F$2:$F$5,0),MATCH(C22,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C22="eSurvey+SMS",ROUND(Q22*INDEX(Lists!$H$3:$H$5,MATCH(B22,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J22" s="8" t="str">
@@ -1901,16 +1901,16 @@
       <c r="D23" s="12"/>
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
-      <c r="G23" s="18" t="str">
+      <c r="G23" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H23" s="8" t="str">
-        <f>IF(ISBLANK(B23),"--",ROUND(P23*INDEX(Lists!$F$2:$H$5,MATCH(B23,Lists!$F$2:$F$5,0),MATCH(C23,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B23),"--",ROUND(P23*INDEX(Lists!$G$3:$G$5,MATCH(B23,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I23" s="7" t="str">
-        <f>IF($C23="eSurvey+SMS",ROUND(Q23*INDEX(Lists!$F$2:$H$5,MATCH(B23,Lists!$F$2:$F$5,0),MATCH(C23,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C23="eSurvey+SMS",ROUND(Q23*INDEX(Lists!$H$3:$H$5,MATCH(B23,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J23" s="8" t="str">
@@ -1958,16 +1958,16 @@
       <c r="D24" s="12"/>
       <c r="E24" s="10"/>
       <c r="F24" s="11"/>
-      <c r="G24" s="18" t="str">
+      <c r="G24" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H24" s="8" t="str">
-        <f>IF(ISBLANK(B24),"--",ROUND(P24*INDEX(Lists!$F$2:$H$5,MATCH(B24,Lists!$F$2:$F$5,0),MATCH(C24,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B24),"--",ROUND(P24*INDEX(Lists!$G$3:$G$5,MATCH(B24,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I24" s="7" t="str">
-        <f>IF($C24="eSurvey+SMS",ROUND(Q24*INDEX(Lists!$F$2:$H$5,MATCH(B24,Lists!$F$2:$F$5,0),MATCH(C24,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C24="eSurvey+SMS",ROUND(Q24*INDEX(Lists!$H$3:$H$5,MATCH(B24,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J24" s="8" t="str">
@@ -2015,16 +2015,16 @@
       <c r="D25" s="12"/>
       <c r="E25" s="10"/>
       <c r="F25" s="11"/>
-      <c r="G25" s="18" t="str">
+      <c r="G25" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H25" s="8" t="str">
-        <f>IF(ISBLANK(B25),"--",ROUND(P25*INDEX(Lists!$F$2:$H$5,MATCH(B25,Lists!$F$2:$F$5,0),MATCH(C25,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B25),"--",ROUND(P25*INDEX(Lists!$G$3:$G$5,MATCH(B25,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I25" s="7" t="str">
-        <f>IF($C25="eSurvey+SMS",ROUND(Q25*INDEX(Lists!$F$2:$H$5,MATCH(B25,Lists!$F$2:$F$5,0),MATCH(C25,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C25="eSurvey+SMS",ROUND(Q25*INDEX(Lists!$H$3:$H$5,MATCH(B25,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J25" s="8" t="str">
@@ -2072,16 +2072,16 @@
       <c r="D26" s="12"/>
       <c r="E26" s="10"/>
       <c r="F26" s="11"/>
-      <c r="G26" s="18" t="str">
+      <c r="G26" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H26" s="8" t="str">
-        <f>IF(ISBLANK(B26),"--",ROUND(P26*INDEX(Lists!$F$2:$H$5,MATCH(B26,Lists!$F$2:$F$5,0),MATCH(C26,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B26),"--",ROUND(P26*INDEX(Lists!$G$3:$G$5,MATCH(B26,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I26" s="7" t="str">
-        <f>IF($C26="eSurvey+SMS",ROUND(Q26*INDEX(Lists!$F$2:$H$5,MATCH(B26,Lists!$F$2:$F$5,0),MATCH(C26,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C26="eSurvey+SMS",ROUND(Q26*INDEX(Lists!$H$3:$H$5,MATCH(B26,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J26" s="8" t="str">
@@ -2129,16 +2129,16 @@
       <c r="D27" s="12"/>
       <c r="E27" s="10"/>
       <c r="F27" s="11"/>
-      <c r="G27" s="18" t="str">
+      <c r="G27" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H27" s="8" t="str">
-        <f>IF(ISBLANK(B27),"--",ROUND(P27*INDEX(Lists!$F$2:$H$5,MATCH(B27,Lists!$F$2:$F$5,0),MATCH(C27,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B27),"--",ROUND(P27*INDEX(Lists!$G$3:$G$5,MATCH(B27,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I27" s="7" t="str">
-        <f>IF($C27="eSurvey+SMS",ROUND(Q27*INDEX(Lists!$F$2:$H$5,MATCH(B27,Lists!$F$2:$F$5,0),MATCH(C27,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C27="eSurvey+SMS",ROUND(Q27*INDEX(Lists!$H$3:$H$5,MATCH(B27,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J27" s="8" t="str">
@@ -2186,16 +2186,16 @@
       <c r="D28" s="12"/>
       <c r="E28" s="10"/>
       <c r="F28" s="11"/>
-      <c r="G28" s="18" t="str">
+      <c r="G28" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H28" s="8" t="str">
-        <f>IF(ISBLANK(B28),"--",ROUND(P28*INDEX(Lists!$F$2:$H$5,MATCH(B28,Lists!$F$2:$F$5,0),MATCH(C28,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B28),"--",ROUND(P28*INDEX(Lists!$G$3:$G$5,MATCH(B28,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I28" s="7" t="str">
-        <f>IF($C28="eSurvey+SMS",ROUND(Q28*INDEX(Lists!$F$2:$H$5,MATCH(B28,Lists!$F$2:$F$5,0),MATCH(C28,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C28="eSurvey+SMS",ROUND(Q28*INDEX(Lists!$H$3:$H$5,MATCH(B28,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J28" s="8" t="str">
@@ -2243,16 +2243,16 @@
       <c r="D29" s="12"/>
       <c r="E29" s="10"/>
       <c r="F29" s="11"/>
-      <c r="G29" s="18" t="str">
+      <c r="G29" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H29" s="8" t="str">
-        <f>IF(ISBLANK(B29),"--",ROUND(P29*INDEX(Lists!$F$2:$H$5,MATCH(B29,Lists!$F$2:$F$5,0),MATCH(C29,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B29),"--",ROUND(P29*INDEX(Lists!$G$3:$G$5,MATCH(B29,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I29" s="7" t="str">
-        <f>IF($C29="eSurvey+SMS",ROUND(Q29*INDEX(Lists!$F$2:$H$5,MATCH(B29,Lists!$F$2:$F$5,0),MATCH(C29,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C29="eSurvey+SMS",ROUND(Q29*INDEX(Lists!$H$3:$H$5,MATCH(B29,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J29" s="8" t="str">
@@ -2300,16 +2300,16 @@
       <c r="D30" s="12"/>
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
-      <c r="G30" s="18" t="str">
+      <c r="G30" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H30" s="8" t="str">
-        <f>IF(ISBLANK(B30),"--",ROUND(P30*INDEX(Lists!$F$2:$H$5,MATCH(B30,Lists!$F$2:$F$5,0),MATCH(C30,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B30),"--",ROUND(P30*INDEX(Lists!$G$3:$G$5,MATCH(B30,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I30" s="7" t="str">
-        <f>IF($C30="eSurvey+SMS",ROUND(Q30*INDEX(Lists!$F$2:$H$5,MATCH(B30,Lists!$F$2:$F$5,0),MATCH(C30,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C30="eSurvey+SMS",ROUND(Q30*INDEX(Lists!$H$3:$H$5,MATCH(B30,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J30" s="8" t="str">
@@ -2357,16 +2357,16 @@
       <c r="D31" s="12"/>
       <c r="E31" s="10"/>
       <c r="F31" s="11"/>
-      <c r="G31" s="18" t="str">
+      <c r="G31" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H31" s="8" t="str">
-        <f>IF(ISBLANK(B31),"--",ROUND(P31*INDEX(Lists!$F$2:$H$5,MATCH(B31,Lists!$F$2:$F$5,0),MATCH(C31,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B31),"--",ROUND(P31*INDEX(Lists!$G$3:$G$5,MATCH(B31,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I31" s="7" t="str">
-        <f>IF($C31="eSurvey+SMS",ROUND(Q31*INDEX(Lists!$F$2:$H$5,MATCH(B31,Lists!$F$2:$F$5,0),MATCH(C31,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C31="eSurvey+SMS",ROUND(Q31*INDEX(Lists!$H$3:$H$5,MATCH(B31,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J31" s="8" t="str">
@@ -2414,16 +2414,16 @@
       <c r="D32" s="12"/>
       <c r="E32" s="10"/>
       <c r="F32" s="11"/>
-      <c r="G32" s="18" t="str">
+      <c r="G32" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H32" s="8" t="str">
-        <f>IF(ISBLANK(B32),"--",ROUND(P32*INDEX(Lists!$F$2:$H$5,MATCH(B32,Lists!$F$2:$F$5,0),MATCH(C32,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B32),"--",ROUND(P32*INDEX(Lists!$G$3:$G$5,MATCH(B32,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I32" s="7" t="str">
-        <f>IF($C32="eSurvey+SMS",ROUND(Q32*INDEX(Lists!$F$2:$H$5,MATCH(B32,Lists!$F$2:$F$5,0),MATCH(C32,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C32="eSurvey+SMS",ROUND(Q32*INDEX(Lists!$H$3:$H$5,MATCH(B32,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J32" s="8" t="str">
@@ -2471,16 +2471,16 @@
       <c r="D33" s="12"/>
       <c r="E33" s="10"/>
       <c r="F33" s="11"/>
-      <c r="G33" s="18" t="str">
+      <c r="G33" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H33" s="8" t="str">
-        <f>IF(ISBLANK(B33),"--",ROUND(P33*INDEX(Lists!$F$2:$H$5,MATCH(B33,Lists!$F$2:$F$5,0),MATCH(C33,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B33),"--",ROUND(P33*INDEX(Lists!$G$3:$G$5,MATCH(B33,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I33" s="7" t="str">
-        <f>IF($C33="eSurvey+SMS",ROUND(Q33*INDEX(Lists!$F$2:$H$5,MATCH(B33,Lists!$F$2:$F$5,0),MATCH(C33,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C33="eSurvey+SMS",ROUND(Q33*INDEX(Lists!$H$3:$H$5,MATCH(B33,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J33" s="8" t="str">
@@ -2528,16 +2528,16 @@
       <c r="D34" s="12"/>
       <c r="E34" s="10"/>
       <c r="F34" s="11"/>
-      <c r="G34" s="18" t="str">
+      <c r="G34" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H34" s="8" t="str">
-        <f>IF(ISBLANK(B34),"--",ROUND(P34*INDEX(Lists!$F$2:$H$5,MATCH(B34,Lists!$F$2:$F$5,0),MATCH(C34,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B34),"--",ROUND(P34*INDEX(Lists!$G$3:$G$5,MATCH(B34,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I34" s="7" t="str">
-        <f>IF($C34="eSurvey+SMS",ROUND(Q34*INDEX(Lists!$F$2:$H$5,MATCH(B34,Lists!$F$2:$F$5,0),MATCH(C34,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C34="eSurvey+SMS",ROUND(Q34*INDEX(Lists!$H$3:$H$5,MATCH(B34,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J34" s="8" t="str">
@@ -2585,16 +2585,16 @@
       <c r="D35" s="12"/>
       <c r="E35" s="10"/>
       <c r="F35" s="11"/>
-      <c r="G35" s="18" t="str">
+      <c r="G35" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H35" s="8" t="str">
-        <f>IF(ISBLANK(B35),"--",ROUND(P35*INDEX(Lists!$F$2:$H$5,MATCH(B35,Lists!$F$2:$F$5,0),MATCH(C35,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B35),"--",ROUND(P35*INDEX(Lists!$G$3:$G$5,MATCH(B35,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I35" s="7" t="str">
-        <f>IF($C35="eSurvey+SMS",ROUND(Q35*INDEX(Lists!$F$2:$H$5,MATCH(B35,Lists!$F$2:$F$5,0),MATCH(C35,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C35="eSurvey+SMS",ROUND(Q35*INDEX(Lists!$H$3:$H$5,MATCH(B35,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J35" s="8" t="str">
@@ -2642,16 +2642,16 @@
       <c r="D36" s="12"/>
       <c r="E36" s="10"/>
       <c r="F36" s="11"/>
-      <c r="G36" s="18" t="str">
+      <c r="G36" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H36" s="8" t="str">
-        <f>IF(ISBLANK(B36),"--",ROUND(P36*INDEX(Lists!$F$2:$H$5,MATCH(B36,Lists!$F$2:$F$5,0),MATCH(C36,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B36),"--",ROUND(P36*INDEX(Lists!$G$3:$G$5,MATCH(B36,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I36" s="7" t="str">
-        <f>IF($C36="eSurvey+SMS",ROUND(Q36*INDEX(Lists!$F$2:$H$5,MATCH(B36,Lists!$F$2:$F$5,0),MATCH(C36,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C36="eSurvey+SMS",ROUND(Q36*INDEX(Lists!$H$3:$H$5,MATCH(B36,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J36" s="8" t="str">
@@ -2699,16 +2699,16 @@
       <c r="D37" s="12"/>
       <c r="E37" s="10"/>
       <c r="F37" s="11"/>
-      <c r="G37" s="18" t="str">
+      <c r="G37" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H37" s="8" t="str">
-        <f>IF(ISBLANK(B37),"--",ROUND(P37*INDEX(Lists!$F$2:$H$5,MATCH(B37,Lists!$F$2:$F$5,0),MATCH(C37,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B37),"--",ROUND(P37*INDEX(Lists!$G$3:$G$5,MATCH(B37,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I37" s="7" t="str">
-        <f>IF($C37="eSurvey+SMS",ROUND(Q37*INDEX(Lists!$F$2:$H$5,MATCH(B37,Lists!$F$2:$F$5,0),MATCH(C37,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C37="eSurvey+SMS",ROUND(Q37*INDEX(Lists!$H$3:$H$5,MATCH(B37,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J37" s="8" t="str">
@@ -2756,16 +2756,16 @@
       <c r="D38" s="12"/>
       <c r="E38" s="10"/>
       <c r="F38" s="11"/>
-      <c r="G38" s="18" t="str">
+      <c r="G38" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H38" s="8" t="str">
-        <f>IF(ISBLANK(B38),"--",ROUND(P38*INDEX(Lists!$F$2:$H$5,MATCH(B38,Lists!$F$2:$F$5,0),MATCH(C38,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B38),"--",ROUND(P38*INDEX(Lists!$G$3:$G$5,MATCH(B38,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I38" s="7" t="str">
-        <f>IF($C38="eSurvey+SMS",ROUND(Q38*INDEX(Lists!$F$2:$H$5,MATCH(B38,Lists!$F$2:$F$5,0),MATCH(C38,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C38="eSurvey+SMS",ROUND(Q38*INDEX(Lists!$H$3:$H$5,MATCH(B38,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J38" s="8" t="str">
@@ -2813,16 +2813,16 @@
       <c r="D39" s="12"/>
       <c r="E39" s="10"/>
       <c r="F39" s="11"/>
-      <c r="G39" s="18" t="str">
+      <c r="G39" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H39" s="8" t="str">
-        <f>IF(ISBLANK(B39),"--",ROUND(P39*INDEX(Lists!$F$2:$H$5,MATCH(B39,Lists!$F$2:$F$5,0),MATCH(C39,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B39),"--",ROUND(P39*INDEX(Lists!$G$3:$G$5,MATCH(B39,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I39" s="7" t="str">
-        <f>IF($C39="eSurvey+SMS",ROUND(Q39*INDEX(Lists!$F$2:$H$5,MATCH(B39,Lists!$F$2:$F$5,0),MATCH(C39,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C39="eSurvey+SMS",ROUND(Q39*INDEX(Lists!$H$3:$H$5,MATCH(B39,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J39" s="8" t="str">
@@ -2870,16 +2870,16 @@
       <c r="D40" s="12"/>
       <c r="E40" s="10"/>
       <c r="F40" s="11"/>
-      <c r="G40" s="18" t="str">
+      <c r="G40" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H40" s="8" t="str">
-        <f>IF(ISBLANK(B40),"--",ROUND(P40*INDEX(Lists!$F$2:$H$5,MATCH(B40,Lists!$F$2:$F$5,0),MATCH(C40,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B40),"--",ROUND(P40*INDEX(Lists!$G$3:$G$5,MATCH(B40,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I40" s="7" t="str">
-        <f>IF($C40="eSurvey+SMS",ROUND(Q40*INDEX(Lists!$F$2:$H$5,MATCH(B40,Lists!$F$2:$F$5,0),MATCH(C40,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C40="eSurvey+SMS",ROUND(Q40*INDEX(Lists!$H$3:$H$5,MATCH(B40,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J40" s="8" t="str">
@@ -2927,16 +2927,16 @@
       <c r="D41" s="12"/>
       <c r="E41" s="10"/>
       <c r="F41" s="11"/>
-      <c r="G41" s="18" t="str">
+      <c r="G41" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H41" s="8" t="str">
-        <f>IF(ISBLANK(B41),"--",ROUND(P41*INDEX(Lists!$F$2:$H$5,MATCH(B41,Lists!$F$2:$F$5,0),MATCH(C41,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B41),"--",ROUND(P41*INDEX(Lists!$G$3:$G$5,MATCH(B41,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I41" s="7" t="str">
-        <f>IF($C41="eSurvey+SMS",ROUND(Q41*INDEX(Lists!$F$2:$H$5,MATCH(B41,Lists!$F$2:$F$5,0),MATCH(C41,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C41="eSurvey+SMS",ROUND(Q41*INDEX(Lists!$H$3:$H$5,MATCH(B41,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J41" s="8" t="str">
@@ -2984,16 +2984,16 @@
       <c r="D42" s="12"/>
       <c r="E42" s="10"/>
       <c r="F42" s="11"/>
-      <c r="G42" s="18" t="str">
+      <c r="G42" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H42" s="8" t="str">
-        <f>IF(ISBLANK(B42),"--",ROUND(P42*INDEX(Lists!$F$2:$H$5,MATCH(B42,Lists!$F$2:$F$5,0),MATCH(C42,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B42),"--",ROUND(P42*INDEX(Lists!$G$3:$G$5,MATCH(B42,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I42" s="7" t="str">
-        <f>IF($C42="eSurvey+SMS",ROUND(Q42*INDEX(Lists!$F$2:$H$5,MATCH(B42,Lists!$F$2:$F$5,0),MATCH(C42,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C42="eSurvey+SMS",ROUND(Q42*INDEX(Lists!$H$3:$H$5,MATCH(B42,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J42" s="8" t="str">
@@ -3041,16 +3041,16 @@
       <c r="D43" s="12"/>
       <c r="E43" s="10"/>
       <c r="F43" s="11"/>
-      <c r="G43" s="18" t="str">
+      <c r="G43" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H43" s="8" t="str">
-        <f>IF(ISBLANK(B43),"--",ROUND(P43*INDEX(Lists!$F$2:$H$5,MATCH(B43,Lists!$F$2:$F$5,0),MATCH(C43,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B43),"--",ROUND(P43*INDEX(Lists!$G$3:$G$5,MATCH(B43,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I43" s="7" t="str">
-        <f>IF($C43="eSurvey+SMS",ROUND(Q43*INDEX(Lists!$F$2:$H$5,MATCH(B43,Lists!$F$2:$F$5,0),MATCH(C43,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C43="eSurvey+SMS",ROUND(Q43*INDEX(Lists!$H$3:$H$5,MATCH(B43,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J43" s="8" t="str">
@@ -3098,16 +3098,16 @@
       <c r="D44" s="12"/>
       <c r="E44" s="10"/>
       <c r="F44" s="11"/>
-      <c r="G44" s="18" t="str">
+      <c r="G44" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H44" s="8" t="str">
-        <f>IF(ISBLANK(B44),"--",ROUND(P44*INDEX(Lists!$F$2:$H$5,MATCH(B44,Lists!$F$2:$F$5,0),MATCH(C44,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B44),"--",ROUND(P44*INDEX(Lists!$G$3:$G$5,MATCH(B44,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I44" s="7" t="str">
-        <f>IF($C44="eSurvey+SMS",ROUND(Q44*INDEX(Lists!$F$2:$H$5,MATCH(B44,Lists!$F$2:$F$5,0),MATCH(C44,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C44="eSurvey+SMS",ROUND(Q44*INDEX(Lists!$H$3:$H$5,MATCH(B44,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J44" s="8" t="str">
@@ -3155,16 +3155,16 @@
       <c r="D45" s="12"/>
       <c r="E45" s="10"/>
       <c r="F45" s="11"/>
-      <c r="G45" s="18" t="str">
+      <c r="G45" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H45" s="8" t="str">
-        <f>IF(ISBLANK(B45),"--",ROUND(P45*INDEX(Lists!$F$2:$H$5,MATCH(B45,Lists!$F$2:$F$5,0),MATCH(C45,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B45),"--",ROUND(P45*INDEX(Lists!$G$3:$G$5,MATCH(B45,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I45" s="7" t="str">
-        <f>IF($C45="eSurvey+SMS",ROUND(Q45*INDEX(Lists!$F$2:$H$5,MATCH(B45,Lists!$F$2:$F$5,0),MATCH(C45,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C45="eSurvey+SMS",ROUND(Q45*INDEX(Lists!$H$3:$H$5,MATCH(B45,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J45" s="8" t="str">
@@ -3212,16 +3212,16 @@
       <c r="D46" s="12"/>
       <c r="E46" s="10"/>
       <c r="F46" s="11"/>
-      <c r="G46" s="18" t="str">
+      <c r="G46" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H46" s="8" t="str">
-        <f>IF(ISBLANK(B46),"--",ROUND(P46*INDEX(Lists!$F$2:$H$5,MATCH(B46,Lists!$F$2:$F$5,0),MATCH(C46,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B46),"--",ROUND(P46*INDEX(Lists!$G$3:$G$5,MATCH(B46,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I46" s="7" t="str">
-        <f>IF($C46="eSurvey+SMS",ROUND(Q46*INDEX(Lists!$F$2:$H$5,MATCH(B46,Lists!$F$2:$F$5,0),MATCH(C46,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C46="eSurvey+SMS",ROUND(Q46*INDEX(Lists!$H$3:$H$5,MATCH(B46,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J46" s="8" t="str">
@@ -3269,16 +3269,16 @@
       <c r="D47" s="12"/>
       <c r="E47" s="10"/>
       <c r="F47" s="11"/>
-      <c r="G47" s="18" t="str">
+      <c r="G47" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H47" s="8" t="str">
-        <f>IF(ISBLANK(B47),"--",ROUND(P47*INDEX(Lists!$F$2:$H$5,MATCH(B47,Lists!$F$2:$F$5,0),MATCH(C47,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B47),"--",ROUND(P47*INDEX(Lists!$G$3:$G$5,MATCH(B47,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I47" s="7" t="str">
-        <f>IF($C47="eSurvey+SMS",ROUND(Q47*INDEX(Lists!$F$2:$H$5,MATCH(B47,Lists!$F$2:$F$5,0),MATCH(C47,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C47="eSurvey+SMS",ROUND(Q47*INDEX(Lists!$H$3:$H$5,MATCH(B47,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J47" s="8" t="str">
@@ -3326,16 +3326,16 @@
       <c r="D48" s="12"/>
       <c r="E48" s="10"/>
       <c r="F48" s="11"/>
-      <c r="G48" s="18" t="str">
+      <c r="G48" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H48" s="8" t="str">
-        <f>IF(ISBLANK(B48),"--",ROUND(P48*INDEX(Lists!$F$2:$H$5,MATCH(B48,Lists!$F$2:$F$5,0),MATCH(C48,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B48),"--",ROUND(P48*INDEX(Lists!$G$3:$G$5,MATCH(B48,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I48" s="7" t="str">
-        <f>IF($C48="eSurvey+SMS",ROUND(Q48*INDEX(Lists!$F$2:$H$5,MATCH(B48,Lists!$F$2:$F$5,0),MATCH(C48,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C48="eSurvey+SMS",ROUND(Q48*INDEX(Lists!$H$3:$H$5,MATCH(B48,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J48" s="8" t="str">
@@ -3383,16 +3383,16 @@
       <c r="D49" s="12"/>
       <c r="E49" s="10"/>
       <c r="F49" s="11"/>
-      <c r="G49" s="18" t="str">
+      <c r="G49" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H49" s="8" t="str">
-        <f>IF(ISBLANK(B49),"--",ROUND(P49*INDEX(Lists!$F$2:$H$5,MATCH(B49,Lists!$F$2:$F$5,0),MATCH(C49,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B49),"--",ROUND(P49*INDEX(Lists!$G$3:$G$5,MATCH(B49,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I49" s="7" t="str">
-        <f>IF($C49="eSurvey+SMS",ROUND(Q49*INDEX(Lists!$F$2:$H$5,MATCH(B49,Lists!$F$2:$F$5,0),MATCH(C49,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C49="eSurvey+SMS",ROUND(Q49*INDEX(Lists!$H$3:$H$5,MATCH(B49,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J49" s="8" t="str">
@@ -3440,16 +3440,16 @@
       <c r="D50" s="12"/>
       <c r="E50" s="10"/>
       <c r="F50" s="11"/>
-      <c r="G50" s="18" t="str">
+      <c r="G50" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H50" s="8" t="str">
-        <f>IF(ISBLANK(B50),"--",ROUND(P50*INDEX(Lists!$F$2:$H$5,MATCH(B50,Lists!$F$2:$F$5,0),MATCH(C50,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B50),"--",ROUND(P50*INDEX(Lists!$G$3:$G$5,MATCH(B50,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I50" s="7" t="str">
-        <f>IF($C50="eSurvey+SMS",ROUND(Q50*INDEX(Lists!$F$2:$H$5,MATCH(B50,Lists!$F$2:$F$5,0),MATCH(C50,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C50="eSurvey+SMS",ROUND(Q50*INDEX(Lists!$H$3:$H$5,MATCH(B50,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J50" s="8" t="str">
@@ -3497,16 +3497,16 @@
       <c r="D51" s="12"/>
       <c r="E51" s="10"/>
       <c r="F51" s="11"/>
-      <c r="G51" s="18" t="str">
+      <c r="G51" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H51" s="8" t="str">
-        <f>IF(ISBLANK(B51),"--",ROUND(P51*INDEX(Lists!$F$2:$H$5,MATCH(B51,Lists!$F$2:$F$5,0),MATCH(C51,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B51),"--",ROUND(P51*INDEX(Lists!$G$3:$G$5,MATCH(B51,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I51" s="7" t="str">
-        <f>IF($C51="eSurvey+SMS",ROUND(Q51*INDEX(Lists!$F$2:$H$5,MATCH(B51,Lists!$F$2:$F$5,0),MATCH(C51,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C51="eSurvey+SMS",ROUND(Q51*INDEX(Lists!$H$3:$H$5,MATCH(B51,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J51" s="8" t="str">
@@ -3554,16 +3554,16 @@
       <c r="D52" s="12"/>
       <c r="E52" s="10"/>
       <c r="F52" s="11"/>
-      <c r="G52" s="18" t="str">
+      <c r="G52" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H52" s="8" t="str">
-        <f>IF(ISBLANK(B52),"--",ROUND(P52*INDEX(Lists!$F$2:$H$5,MATCH(B52,Lists!$F$2:$F$5,0),MATCH(C52,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B52),"--",ROUND(P52*INDEX(Lists!$G$3:$G$5,MATCH(B52,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I52" s="7" t="str">
-        <f>IF($C52="eSurvey+SMS",ROUND(Q52*INDEX(Lists!$F$2:$H$5,MATCH(B52,Lists!$F$2:$F$5,0),MATCH(C52,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C52="eSurvey+SMS",ROUND(Q52*INDEX(Lists!$H$3:$H$5,MATCH(B52,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J52" s="8" t="str">
@@ -3611,16 +3611,16 @@
       <c r="D53" s="12"/>
       <c r="E53" s="10"/>
       <c r="F53" s="11"/>
-      <c r="G53" s="18" t="str">
+      <c r="G53" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H53" s="8" t="str">
-        <f>IF(ISBLANK(B53),"--",ROUND(P53*INDEX(Lists!$F$2:$H$5,MATCH(B53,Lists!$F$2:$F$5,0),MATCH(C53,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B53),"--",ROUND(P53*INDEX(Lists!$G$3:$G$5,MATCH(B53,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I53" s="7" t="str">
-        <f>IF($C53="eSurvey+SMS",ROUND(Q53*INDEX(Lists!$F$2:$H$5,MATCH(B53,Lists!$F$2:$F$5,0),MATCH(C53,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C53="eSurvey+SMS",ROUND(Q53*INDEX(Lists!$H$3:$H$5,MATCH(B53,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J53" s="8" t="str">
@@ -3668,16 +3668,16 @@
       <c r="D54" s="12"/>
       <c r="E54" s="10"/>
       <c r="F54" s="11"/>
-      <c r="G54" s="18" t="str">
+      <c r="G54" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H54" s="8" t="str">
-        <f>IF(ISBLANK(B54),"--",ROUND(P54*INDEX(Lists!$F$2:$H$5,MATCH(B54,Lists!$F$2:$F$5,0),MATCH(C54,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B54),"--",ROUND(P54*INDEX(Lists!$G$3:$G$5,MATCH(B54,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I54" s="7" t="str">
-        <f>IF($C54="eSurvey+SMS",ROUND(Q54*INDEX(Lists!$F$2:$H$5,MATCH(B54,Lists!$F$2:$F$5,0),MATCH(C54,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C54="eSurvey+SMS",ROUND(Q54*INDEX(Lists!$H$3:$H$5,MATCH(B54,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J54" s="8" t="str">
@@ -3725,16 +3725,16 @@
       <c r="D55" s="12"/>
       <c r="E55" s="10"/>
       <c r="F55" s="11"/>
-      <c r="G55" s="18" t="str">
+      <c r="G55" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H55" s="8" t="str">
-        <f>IF(ISBLANK(B55),"--",ROUND(P55*INDEX(Lists!$F$2:$H$5,MATCH(B55,Lists!$F$2:$F$5,0),MATCH(C55,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B55),"--",ROUND(P55*INDEX(Lists!$G$3:$G$5,MATCH(B55,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I55" s="7" t="str">
-        <f>IF($C55="eSurvey+SMS",ROUND(Q55*INDEX(Lists!$F$2:$H$5,MATCH(B55,Lists!$F$2:$F$5,0),MATCH(C55,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C55="eSurvey+SMS",ROUND(Q55*INDEX(Lists!$H$3:$H$5,MATCH(B55,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J55" s="8" t="str">
@@ -3782,16 +3782,16 @@
       <c r="D56" s="12"/>
       <c r="E56" s="10"/>
       <c r="F56" s="11"/>
-      <c r="G56" s="18" t="str">
+      <c r="G56" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H56" s="8" t="str">
-        <f>IF(ISBLANK(B56),"--",ROUND(P56*INDEX(Lists!$F$2:$H$5,MATCH(B56,Lists!$F$2:$F$5,0),MATCH(C56,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B56),"--",ROUND(P56*INDEX(Lists!$G$3:$G$5,MATCH(B56,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I56" s="7" t="str">
-        <f>IF($C56="eSurvey+SMS",ROUND(Q56*INDEX(Lists!$F$2:$H$5,MATCH(B56,Lists!$F$2:$F$5,0),MATCH(C56,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C56="eSurvey+SMS",ROUND(Q56*INDEX(Lists!$H$3:$H$5,MATCH(B56,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J56" s="8" t="str">
@@ -3839,16 +3839,16 @@
       <c r="D57" s="12"/>
       <c r="E57" s="10"/>
       <c r="F57" s="11"/>
-      <c r="G57" s="18" t="str">
+      <c r="G57" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H57" s="8" t="str">
-        <f>IF(ISBLANK(B57),"--",ROUND(P57*INDEX(Lists!$F$2:$H$5,MATCH(B57,Lists!$F$2:$F$5,0),MATCH(C57,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B57),"--",ROUND(P57*INDEX(Lists!$G$3:$G$5,MATCH(B57,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I57" s="7" t="str">
-        <f>IF($C57="eSurvey+SMS",ROUND(Q57*INDEX(Lists!$F$2:$H$5,MATCH(B57,Lists!$F$2:$F$5,0),MATCH(C57,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C57="eSurvey+SMS",ROUND(Q57*INDEX(Lists!$H$3:$H$5,MATCH(B57,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J57" s="8" t="str">
@@ -3896,16 +3896,16 @@
       <c r="D58" s="12"/>
       <c r="E58" s="10"/>
       <c r="F58" s="11"/>
-      <c r="G58" s="18" t="str">
+      <c r="G58" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H58" s="8" t="str">
-        <f>IF(ISBLANK(B58),"--",ROUND(P58*INDEX(Lists!$F$2:$H$5,MATCH(B58,Lists!$F$2:$F$5,0),MATCH(C58,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B58),"--",ROUND(P58*INDEX(Lists!$G$3:$G$5,MATCH(B58,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I58" s="7" t="str">
-        <f>IF($C58="eSurvey+SMS",ROUND(Q58*INDEX(Lists!$F$2:$H$5,MATCH(B58,Lists!$F$2:$F$5,0),MATCH(C58,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C58="eSurvey+SMS",ROUND(Q58*INDEX(Lists!$H$3:$H$5,MATCH(B58,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J58" s="8" t="str">
@@ -3953,16 +3953,16 @@
       <c r="D59" s="12"/>
       <c r="E59" s="10"/>
       <c r="F59" s="11"/>
-      <c r="G59" s="18" t="str">
+      <c r="G59" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H59" s="8" t="str">
-        <f>IF(ISBLANK(B59),"--",ROUND(P59*INDEX(Lists!$F$2:$H$5,MATCH(B59,Lists!$F$2:$F$5,0),MATCH(C59,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B59),"--",ROUND(P59*INDEX(Lists!$G$3:$G$5,MATCH(B59,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I59" s="7" t="str">
-        <f>IF($C59="eSurvey+SMS",ROUND(Q59*INDEX(Lists!$F$2:$H$5,MATCH(B59,Lists!$F$2:$F$5,0),MATCH(C59,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C59="eSurvey+SMS",ROUND(Q59*INDEX(Lists!$H$3:$H$5,MATCH(B59,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J59" s="8" t="str">
@@ -4010,16 +4010,16 @@
       <c r="D60" s="12"/>
       <c r="E60" s="10"/>
       <c r="F60" s="11"/>
-      <c r="G60" s="18" t="str">
+      <c r="G60" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H60" s="8" t="str">
-        <f>IF(ISBLANK(B60),"--",ROUND(P60*INDEX(Lists!$F$2:$H$5,MATCH(B60,Lists!$F$2:$F$5,0),MATCH(C60,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B60),"--",ROUND(P60*INDEX(Lists!$G$3:$G$5,MATCH(B60,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I60" s="7" t="str">
-        <f>IF($C60="eSurvey+SMS",ROUND(Q60*INDEX(Lists!$F$2:$H$5,MATCH(B60,Lists!$F$2:$F$5,0),MATCH(C60,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C60="eSurvey+SMS",ROUND(Q60*INDEX(Lists!$H$3:$H$5,MATCH(B60,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J60" s="8" t="str">
@@ -4067,16 +4067,16 @@
       <c r="D61" s="12"/>
       <c r="E61" s="10"/>
       <c r="F61" s="11"/>
-      <c r="G61" s="18" t="str">
+      <c r="G61" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H61" s="8" t="str">
-        <f>IF(ISBLANK(B61),"--",ROUND(P61*INDEX(Lists!$F$2:$H$5,MATCH(B61,Lists!$F$2:$F$5,0),MATCH(C61,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B61),"--",ROUND(P61*INDEX(Lists!$G$3:$G$5,MATCH(B61,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I61" s="7" t="str">
-        <f>IF($C61="eSurvey+SMS",ROUND(Q61*INDEX(Lists!$F$2:$H$5,MATCH(B61,Lists!$F$2:$F$5,0),MATCH(C61,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C61="eSurvey+SMS",ROUND(Q61*INDEX(Lists!$H$3:$H$5,MATCH(B61,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J61" s="8" t="str">
@@ -4124,16 +4124,16 @@
       <c r="D62" s="12"/>
       <c r="E62" s="10"/>
       <c r="F62" s="11"/>
-      <c r="G62" s="18" t="str">
+      <c r="G62" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H62" s="8" t="str">
-        <f>IF(ISBLANK(B62),"--",ROUND(P62*INDEX(Lists!$F$2:$H$5,MATCH(B62,Lists!$F$2:$F$5,0),MATCH(C62,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B62),"--",ROUND(P62*INDEX(Lists!$G$3:$G$5,MATCH(B62,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I62" s="7" t="str">
-        <f>IF($C62="eSurvey+SMS",ROUND(Q62*INDEX(Lists!$F$2:$H$5,MATCH(B62,Lists!$F$2:$F$5,0),MATCH(C62,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C62="eSurvey+SMS",ROUND(Q62*INDEX(Lists!$H$3:$H$5,MATCH(B62,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J62" s="8" t="str">
@@ -4181,16 +4181,16 @@
       <c r="D63" s="12"/>
       <c r="E63" s="10"/>
       <c r="F63" s="11"/>
-      <c r="G63" s="18" t="str">
+      <c r="G63" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H63" s="8" t="str">
-        <f>IF(ISBLANK(B63),"--",ROUND(P63*INDEX(Lists!$F$2:$H$5,MATCH(B63,Lists!$F$2:$F$5,0),MATCH(C63,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B63),"--",ROUND(P63*INDEX(Lists!$G$3:$G$5,MATCH(B63,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I63" s="7" t="str">
-        <f>IF($C63="eSurvey+SMS",ROUND(Q63*INDEX(Lists!$F$2:$H$5,MATCH(B63,Lists!$F$2:$F$5,0),MATCH(C63,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C63="eSurvey+SMS",ROUND(Q63*INDEX(Lists!$H$3:$H$5,MATCH(B63,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J63" s="8" t="str">
@@ -4238,16 +4238,16 @@
       <c r="D64" s="12"/>
       <c r="E64" s="10"/>
       <c r="F64" s="11"/>
-      <c r="G64" s="18" t="str">
+      <c r="G64" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H64" s="8" t="str">
-        <f>IF(ISBLANK(B64),"--",ROUND(P64*INDEX(Lists!$F$2:$H$5,MATCH(B64,Lists!$F$2:$F$5,0),MATCH(C64,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B64),"--",ROUND(P64*INDEX(Lists!$G$3:$G$5,MATCH(B64,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I64" s="7" t="str">
-        <f>IF($C64="eSurvey+SMS",ROUND(Q64*INDEX(Lists!$F$2:$H$5,MATCH(B64,Lists!$F$2:$F$5,0),MATCH(C64,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C64="eSurvey+SMS",ROUND(Q64*INDEX(Lists!$H$3:$H$5,MATCH(B64,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J64" s="8" t="str">
@@ -4295,16 +4295,16 @@
       <c r="D65" s="12"/>
       <c r="E65" s="10"/>
       <c r="F65" s="11"/>
-      <c r="G65" s="18" t="str">
+      <c r="G65" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H65" s="8" t="str">
-        <f>IF(ISBLANK(B65),"--",ROUND(P65*INDEX(Lists!$F$2:$H$5,MATCH(B65,Lists!$F$2:$F$5,0),MATCH(C65,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B65),"--",ROUND(P65*INDEX(Lists!$G$3:$G$5,MATCH(B65,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I65" s="7" t="str">
-        <f>IF($C65="eSurvey+SMS",ROUND(Q65*INDEX(Lists!$F$2:$H$5,MATCH(B65,Lists!$F$2:$F$5,0),MATCH(C65,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C65="eSurvey+SMS",ROUND(Q65*INDEX(Lists!$H$3:$H$5,MATCH(B65,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J65" s="8" t="str">
@@ -4352,16 +4352,16 @@
       <c r="D66" s="12"/>
       <c r="E66" s="10"/>
       <c r="F66" s="11"/>
-      <c r="G66" s="18" t="str">
+      <c r="G66" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H66" s="8" t="str">
-        <f>IF(ISBLANK(B66),"--",ROUND(P66*INDEX(Lists!$F$2:$H$5,MATCH(B66,Lists!$F$2:$F$5,0),MATCH(C66,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B66),"--",ROUND(P66*INDEX(Lists!$G$3:$G$5,MATCH(B66,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I66" s="7" t="str">
-        <f>IF($C66="eSurvey+SMS",ROUND(Q66*INDEX(Lists!$F$2:$H$5,MATCH(B66,Lists!$F$2:$F$5,0),MATCH(C66,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C66="eSurvey+SMS",ROUND(Q66*INDEX(Lists!$H$3:$H$5,MATCH(B66,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J66" s="8" t="str">
@@ -4409,16 +4409,16 @@
       <c r="D67" s="12"/>
       <c r="E67" s="10"/>
       <c r="F67" s="11"/>
-      <c r="G67" s="18" t="str">
+      <c r="G67" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H67" s="8" t="str">
-        <f>IF(ISBLANK(B67),"--",ROUND(P67*INDEX(Lists!$F$2:$H$5,MATCH(B67,Lists!$F$2:$F$5,0),MATCH(C67,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B67),"--",ROUND(P67*INDEX(Lists!$G$3:$G$5,MATCH(B67,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I67" s="7" t="str">
-        <f>IF($C67="eSurvey+SMS",ROUND(Q67*INDEX(Lists!$F$2:$H$5,MATCH(B67,Lists!$F$2:$F$5,0),MATCH(C67,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C67="eSurvey+SMS",ROUND(Q67*INDEX(Lists!$H$3:$H$5,MATCH(B67,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J67" s="8" t="str">
@@ -4466,16 +4466,16 @@
       <c r="D68" s="12"/>
       <c r="E68" s="10"/>
       <c r="F68" s="11"/>
-      <c r="G68" s="18" t="str">
+      <c r="G68" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H68" s="8" t="str">
-        <f>IF(ISBLANK(B68),"--",ROUND(P68*INDEX(Lists!$F$2:$H$5,MATCH(B68,Lists!$F$2:$F$5,0),MATCH(C68,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B68),"--",ROUND(P68*INDEX(Lists!$G$3:$G$5,MATCH(B68,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I68" s="7" t="str">
-        <f>IF($C68="eSurvey+SMS",ROUND(Q68*INDEX(Lists!$F$2:$H$5,MATCH(B68,Lists!$F$2:$F$5,0),MATCH(C68,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C68="eSurvey+SMS",ROUND(Q68*INDEX(Lists!$H$3:$H$5,MATCH(B68,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J68" s="8" t="str">
@@ -4523,16 +4523,16 @@
       <c r="D69" s="12"/>
       <c r="E69" s="10"/>
       <c r="F69" s="11"/>
-      <c r="G69" s="18" t="str">
+      <c r="G69" s="16" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="H69" s="8" t="str">
-        <f>IF(ISBLANK(B69),"--",ROUND(P69*INDEX(Lists!$F$2:$H$5,MATCH(B69,Lists!$F$2:$F$5,0),MATCH(C69,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B69),"--",ROUND(P69*INDEX(Lists!$G$3:$G$5,MATCH(B69,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I69" s="7" t="str">
-        <f>IF($C69="eSurvey+SMS",ROUND(Q69*INDEX(Lists!$F$2:$H$5,MATCH(B69,Lists!$F$2:$F$5,0),MATCH(C69,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C69="eSurvey+SMS",ROUND(Q69*INDEX(Lists!$H$3:$H$5,MATCH(B69,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J69" s="8" t="str">
@@ -4580,16 +4580,16 @@
       <c r="D70" s="12"/>
       <c r="E70" s="10"/>
       <c r="F70" s="11"/>
-      <c r="G70" s="18" t="str">
+      <c r="G70" s="16" t="str">
         <f t="shared" ref="G70:G133" si="8">IF(ISBLANK(B70),"--",SUM(H70,I70))</f>
         <v>--</v>
       </c>
       <c r="H70" s="8" t="str">
-        <f>IF(ISBLANK(B70),"--",ROUND(P70*INDEX(Lists!$F$2:$H$5,MATCH(B70,Lists!$F$2:$F$5,0),MATCH(C70,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B70),"--",ROUND(P70*INDEX(Lists!$G$3:$G$5,MATCH(B70,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I70" s="7" t="str">
-        <f>IF($C70="eSurvey+SMS",ROUND(Q70*INDEX(Lists!$F$2:$H$5,MATCH(B70,Lists!$F$2:$F$5,0),MATCH(C70,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C70="eSurvey+SMS",ROUND(Q70*INDEX(Lists!$H$3:$H$5,MATCH(B70,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J70" s="8" t="str">
@@ -4637,16 +4637,16 @@
       <c r="D71" s="12"/>
       <c r="E71" s="10"/>
       <c r="F71" s="11"/>
-      <c r="G71" s="18" t="str">
+      <c r="G71" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H71" s="8" t="str">
-        <f>IF(ISBLANK(B71),"--",ROUND(P71*INDEX(Lists!$F$2:$H$5,MATCH(B71,Lists!$F$2:$F$5,0),MATCH(C71,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B71),"--",ROUND(P71*INDEX(Lists!$G$3:$G$5,MATCH(B71,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I71" s="7" t="str">
-        <f>IF($C71="eSurvey+SMS",ROUND(Q71*INDEX(Lists!$F$2:$H$5,MATCH(B71,Lists!$F$2:$F$5,0),MATCH(C71,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C71="eSurvey+SMS",ROUND(Q71*INDEX(Lists!$H$3:$H$5,MATCH(B71,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J71" s="8" t="str">
@@ -4694,16 +4694,16 @@
       <c r="D72" s="12"/>
       <c r="E72" s="10"/>
       <c r="F72" s="11"/>
-      <c r="G72" s="18" t="str">
+      <c r="G72" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H72" s="8" t="str">
-        <f>IF(ISBLANK(B72),"--",ROUND(P72*INDEX(Lists!$F$2:$H$5,MATCH(B72,Lists!$F$2:$F$5,0),MATCH(C72,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B72),"--",ROUND(P72*INDEX(Lists!$G$3:$G$5,MATCH(B72,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I72" s="7" t="str">
-        <f>IF($C72="eSurvey+SMS",ROUND(Q72*INDEX(Lists!$F$2:$H$5,MATCH(B72,Lists!$F$2:$F$5,0),MATCH(C72,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C72="eSurvey+SMS",ROUND(Q72*INDEX(Lists!$H$3:$H$5,MATCH(B72,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J72" s="8" t="str">
@@ -4751,16 +4751,16 @@
       <c r="D73" s="12"/>
       <c r="E73" s="10"/>
       <c r="F73" s="11"/>
-      <c r="G73" s="18" t="str">
+      <c r="G73" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H73" s="8" t="str">
-        <f>IF(ISBLANK(B73),"--",ROUND(P73*INDEX(Lists!$F$2:$H$5,MATCH(B73,Lists!$F$2:$F$5,0),MATCH(C73,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B73),"--",ROUND(P73*INDEX(Lists!$G$3:$G$5,MATCH(B73,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I73" s="7" t="str">
-        <f>IF($C73="eSurvey+SMS",ROUND(Q73*INDEX(Lists!$F$2:$H$5,MATCH(B73,Lists!$F$2:$F$5,0),MATCH(C73,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C73="eSurvey+SMS",ROUND(Q73*INDEX(Lists!$H$3:$H$5,MATCH(B73,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J73" s="8" t="str">
@@ -4808,16 +4808,16 @@
       <c r="D74" s="12"/>
       <c r="E74" s="10"/>
       <c r="F74" s="11"/>
-      <c r="G74" s="18" t="str">
+      <c r="G74" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H74" s="8" t="str">
-        <f>IF(ISBLANK(B74),"--",ROUND(P74*INDEX(Lists!$F$2:$H$5,MATCH(B74,Lists!$F$2:$F$5,0),MATCH(C74,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B74),"--",ROUND(P74*INDEX(Lists!$G$3:$G$5,MATCH(B74,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I74" s="7" t="str">
-        <f>IF($C74="eSurvey+SMS",ROUND(Q74*INDEX(Lists!$F$2:$H$5,MATCH(B74,Lists!$F$2:$F$5,0),MATCH(C74,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C74="eSurvey+SMS",ROUND(Q74*INDEX(Lists!$H$3:$H$5,MATCH(B74,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J74" s="8" t="str">
@@ -4865,16 +4865,16 @@
       <c r="D75" s="12"/>
       <c r="E75" s="10"/>
       <c r="F75" s="11"/>
-      <c r="G75" s="18" t="str">
+      <c r="G75" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H75" s="8" t="str">
-        <f>IF(ISBLANK(B75),"--",ROUND(P75*INDEX(Lists!$F$2:$H$5,MATCH(B75,Lists!$F$2:$F$5,0),MATCH(C75,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B75),"--",ROUND(P75*INDEX(Lists!$G$3:$G$5,MATCH(B75,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I75" s="7" t="str">
-        <f>IF($C75="eSurvey+SMS",ROUND(Q75*INDEX(Lists!$F$2:$H$5,MATCH(B75,Lists!$F$2:$F$5,0),MATCH(C75,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C75="eSurvey+SMS",ROUND(Q75*INDEX(Lists!$H$3:$H$5,MATCH(B75,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J75" s="8" t="str">
@@ -4922,16 +4922,16 @@
       <c r="D76" s="12"/>
       <c r="E76" s="10"/>
       <c r="F76" s="11"/>
-      <c r="G76" s="18" t="str">
+      <c r="G76" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H76" s="8" t="str">
-        <f>IF(ISBLANK(B76),"--",ROUND(P76*INDEX(Lists!$F$2:$H$5,MATCH(B76,Lists!$F$2:$F$5,0),MATCH(C76,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B76),"--",ROUND(P76*INDEX(Lists!$G$3:$G$5,MATCH(B76,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I76" s="7" t="str">
-        <f>IF($C76="eSurvey+SMS",ROUND(Q76*INDEX(Lists!$F$2:$H$5,MATCH(B76,Lists!$F$2:$F$5,0),MATCH(C76,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C76="eSurvey+SMS",ROUND(Q76*INDEX(Lists!$H$3:$H$5,MATCH(B76,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J76" s="8" t="str">
@@ -4979,16 +4979,16 @@
       <c r="D77" s="12"/>
       <c r="E77" s="10"/>
       <c r="F77" s="11"/>
-      <c r="G77" s="18" t="str">
+      <c r="G77" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H77" s="8" t="str">
-        <f>IF(ISBLANK(B77),"--",ROUND(P77*INDEX(Lists!$F$2:$H$5,MATCH(B77,Lists!$F$2:$F$5,0),MATCH(C77,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B77),"--",ROUND(P77*INDEX(Lists!$G$3:$G$5,MATCH(B77,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I77" s="7" t="str">
-        <f>IF($C77="eSurvey+SMS",ROUND(Q77*INDEX(Lists!$F$2:$H$5,MATCH(B77,Lists!$F$2:$F$5,0),MATCH(C77,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C77="eSurvey+SMS",ROUND(Q77*INDEX(Lists!$H$3:$H$5,MATCH(B77,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J77" s="8" t="str">
@@ -5036,16 +5036,16 @@
       <c r="D78" s="12"/>
       <c r="E78" s="10"/>
       <c r="F78" s="11"/>
-      <c r="G78" s="18" t="str">
+      <c r="G78" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H78" s="8" t="str">
-        <f>IF(ISBLANK(B78),"--",ROUND(P78*INDEX(Lists!$F$2:$H$5,MATCH(B78,Lists!$F$2:$F$5,0),MATCH(C78,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B78),"--",ROUND(P78*INDEX(Lists!$G$3:$G$5,MATCH(B78,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I78" s="7" t="str">
-        <f>IF($C78="eSurvey+SMS",ROUND(Q78*INDEX(Lists!$F$2:$H$5,MATCH(B78,Lists!$F$2:$F$5,0),MATCH(C78,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C78="eSurvey+SMS",ROUND(Q78*INDEX(Lists!$H$3:$H$5,MATCH(B78,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J78" s="8" t="str">
@@ -5093,16 +5093,16 @@
       <c r="D79" s="12"/>
       <c r="E79" s="10"/>
       <c r="F79" s="11"/>
-      <c r="G79" s="18" t="str">
+      <c r="G79" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H79" s="8" t="str">
-        <f>IF(ISBLANK(B79),"--",ROUND(P79*INDEX(Lists!$F$2:$H$5,MATCH(B79,Lists!$F$2:$F$5,0),MATCH(C79,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B79),"--",ROUND(P79*INDEX(Lists!$G$3:$G$5,MATCH(B79,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I79" s="7" t="str">
-        <f>IF($C79="eSurvey+SMS",ROUND(Q79*INDEX(Lists!$F$2:$H$5,MATCH(B79,Lists!$F$2:$F$5,0),MATCH(C79,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C79="eSurvey+SMS",ROUND(Q79*INDEX(Lists!$H$3:$H$5,MATCH(B79,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J79" s="8" t="str">
@@ -5150,16 +5150,16 @@
       <c r="D80" s="12"/>
       <c r="E80" s="10"/>
       <c r="F80" s="11"/>
-      <c r="G80" s="18" t="str">
+      <c r="G80" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H80" s="8" t="str">
-        <f>IF(ISBLANK(B80),"--",ROUND(P80*INDEX(Lists!$F$2:$H$5,MATCH(B80,Lists!$F$2:$F$5,0),MATCH(C80,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B80),"--",ROUND(P80*INDEX(Lists!$G$3:$G$5,MATCH(B80,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I80" s="7" t="str">
-        <f>IF($C80="eSurvey+SMS",ROUND(Q80*INDEX(Lists!$F$2:$H$5,MATCH(B80,Lists!$F$2:$F$5,0),MATCH(C80,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C80="eSurvey+SMS",ROUND(Q80*INDEX(Lists!$H$3:$H$5,MATCH(B80,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J80" s="8" t="str">
@@ -5207,16 +5207,16 @@
       <c r="D81" s="12"/>
       <c r="E81" s="10"/>
       <c r="F81" s="11"/>
-      <c r="G81" s="18" t="str">
+      <c r="G81" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H81" s="8" t="str">
-        <f>IF(ISBLANK(B81),"--",ROUND(P81*INDEX(Lists!$F$2:$H$5,MATCH(B81,Lists!$F$2:$F$5,0),MATCH(C81,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B81),"--",ROUND(P81*INDEX(Lists!$G$3:$G$5,MATCH(B81,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I81" s="7" t="str">
-        <f>IF($C81="eSurvey+SMS",ROUND(Q81*INDEX(Lists!$F$2:$H$5,MATCH(B81,Lists!$F$2:$F$5,0),MATCH(C81,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C81="eSurvey+SMS",ROUND(Q81*INDEX(Lists!$H$3:$H$5,MATCH(B81,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J81" s="8" t="str">
@@ -5264,16 +5264,16 @@
       <c r="D82" s="12"/>
       <c r="E82" s="10"/>
       <c r="F82" s="11"/>
-      <c r="G82" s="18" t="str">
+      <c r="G82" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H82" s="8" t="str">
-        <f>IF(ISBLANK(B82),"--",ROUND(P82*INDEX(Lists!$F$2:$H$5,MATCH(B82,Lists!$F$2:$F$5,0),MATCH(C82,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B82),"--",ROUND(P82*INDEX(Lists!$G$3:$G$5,MATCH(B82,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I82" s="7" t="str">
-        <f>IF($C82="eSurvey+SMS",ROUND(Q82*INDEX(Lists!$F$2:$H$5,MATCH(B82,Lists!$F$2:$F$5,0),MATCH(C82,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C82="eSurvey+SMS",ROUND(Q82*INDEX(Lists!$H$3:$H$5,MATCH(B82,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J82" s="8" t="str">
@@ -5321,16 +5321,16 @@
       <c r="D83" s="12"/>
       <c r="E83" s="10"/>
       <c r="F83" s="11"/>
-      <c r="G83" s="18" t="str">
+      <c r="G83" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H83" s="8" t="str">
-        <f>IF(ISBLANK(B83),"--",ROUND(P83*INDEX(Lists!$F$2:$H$5,MATCH(B83,Lists!$F$2:$F$5,0),MATCH(C83,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B83),"--",ROUND(P83*INDEX(Lists!$G$3:$G$5,MATCH(B83,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I83" s="7" t="str">
-        <f>IF($C83="eSurvey+SMS",ROUND(Q83*INDEX(Lists!$F$2:$H$5,MATCH(B83,Lists!$F$2:$F$5,0),MATCH(C83,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C83="eSurvey+SMS",ROUND(Q83*INDEX(Lists!$H$3:$H$5,MATCH(B83,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J83" s="8" t="str">
@@ -5378,16 +5378,16 @@
       <c r="D84" s="12"/>
       <c r="E84" s="10"/>
       <c r="F84" s="11"/>
-      <c r="G84" s="18" t="str">
+      <c r="G84" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H84" s="8" t="str">
-        <f>IF(ISBLANK(B84),"--",ROUND(P84*INDEX(Lists!$F$2:$H$5,MATCH(B84,Lists!$F$2:$F$5,0),MATCH(C84,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B84),"--",ROUND(P84*INDEX(Lists!$G$3:$G$5,MATCH(B84,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I84" s="7" t="str">
-        <f>IF($C84="eSurvey+SMS",ROUND(Q84*INDEX(Lists!$F$2:$H$5,MATCH(B84,Lists!$F$2:$F$5,0),MATCH(C84,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C84="eSurvey+SMS",ROUND(Q84*INDEX(Lists!$H$3:$H$5,MATCH(B84,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J84" s="8" t="str">
@@ -5435,16 +5435,16 @@
       <c r="D85" s="12"/>
       <c r="E85" s="10"/>
       <c r="F85" s="11"/>
-      <c r="G85" s="18" t="str">
+      <c r="G85" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H85" s="8" t="str">
-        <f>IF(ISBLANK(B85),"--",ROUND(P85*INDEX(Lists!$F$2:$H$5,MATCH(B85,Lists!$F$2:$F$5,0),MATCH(C85,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B85),"--",ROUND(P85*INDEX(Lists!$G$3:$G$5,MATCH(B85,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I85" s="7" t="str">
-        <f>IF($C85="eSurvey+SMS",ROUND(Q85*INDEX(Lists!$F$2:$H$5,MATCH(B85,Lists!$F$2:$F$5,0),MATCH(C85,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C85="eSurvey+SMS",ROUND(Q85*INDEX(Lists!$H$3:$H$5,MATCH(B85,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J85" s="8" t="str">
@@ -5492,16 +5492,16 @@
       <c r="D86" s="12"/>
       <c r="E86" s="10"/>
       <c r="F86" s="11"/>
-      <c r="G86" s="18" t="str">
+      <c r="G86" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H86" s="8" t="str">
-        <f>IF(ISBLANK(B86),"--",ROUND(P86*INDEX(Lists!$F$2:$H$5,MATCH(B86,Lists!$F$2:$F$5,0),MATCH(C86,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B86),"--",ROUND(P86*INDEX(Lists!$G$3:$G$5,MATCH(B86,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I86" s="7" t="str">
-        <f>IF($C86="eSurvey+SMS",ROUND(Q86*INDEX(Lists!$F$2:$H$5,MATCH(B86,Lists!$F$2:$F$5,0),MATCH(C86,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C86="eSurvey+SMS",ROUND(Q86*INDEX(Lists!$H$3:$H$5,MATCH(B86,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J86" s="8" t="str">
@@ -5549,16 +5549,16 @@
       <c r="D87" s="12"/>
       <c r="E87" s="10"/>
       <c r="F87" s="11"/>
-      <c r="G87" s="18" t="str">
+      <c r="G87" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H87" s="8" t="str">
-        <f>IF(ISBLANK(B87),"--",ROUND(P87*INDEX(Lists!$F$2:$H$5,MATCH(B87,Lists!$F$2:$F$5,0),MATCH(C87,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B87),"--",ROUND(P87*INDEX(Lists!$G$3:$G$5,MATCH(B87,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I87" s="7" t="str">
-        <f>IF($C87="eSurvey+SMS",ROUND(Q87*INDEX(Lists!$F$2:$H$5,MATCH(B87,Lists!$F$2:$F$5,0),MATCH(C87,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C87="eSurvey+SMS",ROUND(Q87*INDEX(Lists!$H$3:$H$5,MATCH(B87,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J87" s="8" t="str">
@@ -5606,16 +5606,16 @@
       <c r="D88" s="12"/>
       <c r="E88" s="10"/>
       <c r="F88" s="11"/>
-      <c r="G88" s="18" t="str">
+      <c r="G88" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H88" s="8" t="str">
-        <f>IF(ISBLANK(B88),"--",ROUND(P88*INDEX(Lists!$F$2:$H$5,MATCH(B88,Lists!$F$2:$F$5,0),MATCH(C88,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B88),"--",ROUND(P88*INDEX(Lists!$G$3:$G$5,MATCH(B88,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I88" s="7" t="str">
-        <f>IF($C88="eSurvey+SMS",ROUND(Q88*INDEX(Lists!$F$2:$H$5,MATCH(B88,Lists!$F$2:$F$5,0),MATCH(C88,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C88="eSurvey+SMS",ROUND(Q88*INDEX(Lists!$H$3:$H$5,MATCH(B88,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J88" s="8" t="str">
@@ -5663,16 +5663,16 @@
       <c r="D89" s="12"/>
       <c r="E89" s="10"/>
       <c r="F89" s="11"/>
-      <c r="G89" s="18" t="str">
+      <c r="G89" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H89" s="8" t="str">
-        <f>IF(ISBLANK(B89),"--",ROUND(P89*INDEX(Lists!$F$2:$H$5,MATCH(B89,Lists!$F$2:$F$5,0),MATCH(C89,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B89),"--",ROUND(P89*INDEX(Lists!$G$3:$G$5,MATCH(B89,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I89" s="7" t="str">
-        <f>IF($C89="eSurvey+SMS",ROUND(Q89*INDEX(Lists!$F$2:$H$5,MATCH(B89,Lists!$F$2:$F$5,0),MATCH(C89,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C89="eSurvey+SMS",ROUND(Q89*INDEX(Lists!$H$3:$H$5,MATCH(B89,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J89" s="8" t="str">
@@ -5720,16 +5720,16 @@
       <c r="D90" s="12"/>
       <c r="E90" s="10"/>
       <c r="F90" s="11"/>
-      <c r="G90" s="18" t="str">
+      <c r="G90" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H90" s="8" t="str">
-        <f>IF(ISBLANK(B90),"--",ROUND(P90*INDEX(Lists!$F$2:$H$5,MATCH(B90,Lists!$F$2:$F$5,0),MATCH(C90,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B90),"--",ROUND(P90*INDEX(Lists!$G$3:$G$5,MATCH(B90,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I90" s="7" t="str">
-        <f>IF($C90="eSurvey+SMS",ROUND(Q90*INDEX(Lists!$F$2:$H$5,MATCH(B90,Lists!$F$2:$F$5,0),MATCH(C90,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C90="eSurvey+SMS",ROUND(Q90*INDEX(Lists!$H$3:$H$5,MATCH(B90,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J90" s="8" t="str">
@@ -5777,16 +5777,16 @@
       <c r="D91" s="12"/>
       <c r="E91" s="10"/>
       <c r="F91" s="11"/>
-      <c r="G91" s="18" t="str">
+      <c r="G91" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H91" s="8" t="str">
-        <f>IF(ISBLANK(B91),"--",ROUND(P91*INDEX(Lists!$F$2:$H$5,MATCH(B91,Lists!$F$2:$F$5,0),MATCH(C91,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B91),"--",ROUND(P91*INDEX(Lists!$G$3:$G$5,MATCH(B91,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I91" s="7" t="str">
-        <f>IF($C91="eSurvey+SMS",ROUND(Q91*INDEX(Lists!$F$2:$H$5,MATCH(B91,Lists!$F$2:$F$5,0),MATCH(C91,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C91="eSurvey+SMS",ROUND(Q91*INDEX(Lists!$H$3:$H$5,MATCH(B91,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J91" s="8" t="str">
@@ -5834,16 +5834,16 @@
       <c r="D92" s="12"/>
       <c r="E92" s="10"/>
       <c r="F92" s="11"/>
-      <c r="G92" s="18" t="str">
+      <c r="G92" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H92" s="8" t="str">
-        <f>IF(ISBLANK(B92),"--",ROUND(P92*INDEX(Lists!$F$2:$H$5,MATCH(B92,Lists!$F$2:$F$5,0),MATCH(C92,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B92),"--",ROUND(P92*INDEX(Lists!$G$3:$G$5,MATCH(B92,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I92" s="7" t="str">
-        <f>IF($C92="eSurvey+SMS",ROUND(Q92*INDEX(Lists!$F$2:$H$5,MATCH(B92,Lists!$F$2:$F$5,0),MATCH(C92,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C92="eSurvey+SMS",ROUND(Q92*INDEX(Lists!$H$3:$H$5,MATCH(B92,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J92" s="8" t="str">
@@ -5891,16 +5891,16 @@
       <c r="D93" s="12"/>
       <c r="E93" s="10"/>
       <c r="F93" s="11"/>
-      <c r="G93" s="18" t="str">
+      <c r="G93" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H93" s="8" t="str">
-        <f>IF(ISBLANK(B93),"--",ROUND(P93*INDEX(Lists!$F$2:$H$5,MATCH(B93,Lists!$F$2:$F$5,0),MATCH(C93,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B93),"--",ROUND(P93*INDEX(Lists!$G$3:$G$5,MATCH(B93,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I93" s="7" t="str">
-        <f>IF($C93="eSurvey+SMS",ROUND(Q93*INDEX(Lists!$F$2:$H$5,MATCH(B93,Lists!$F$2:$F$5,0),MATCH(C93,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C93="eSurvey+SMS",ROUND(Q93*INDEX(Lists!$H$3:$H$5,MATCH(B93,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J93" s="8" t="str">
@@ -5948,16 +5948,16 @@
       <c r="D94" s="12"/>
       <c r="E94" s="10"/>
       <c r="F94" s="11"/>
-      <c r="G94" s="18" t="str">
+      <c r="G94" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H94" s="8" t="str">
-        <f>IF(ISBLANK(B94),"--",ROUND(P94*INDEX(Lists!$F$2:$H$5,MATCH(B94,Lists!$F$2:$F$5,0),MATCH(C94,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B94),"--",ROUND(P94*INDEX(Lists!$G$3:$G$5,MATCH(B94,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I94" s="7" t="str">
-        <f>IF($C94="eSurvey+SMS",ROUND(Q94*INDEX(Lists!$F$2:$H$5,MATCH(B94,Lists!$F$2:$F$5,0),MATCH(C94,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C94="eSurvey+SMS",ROUND(Q94*INDEX(Lists!$H$3:$H$5,MATCH(B94,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J94" s="8" t="str">
@@ -6005,16 +6005,16 @@
       <c r="D95" s="12"/>
       <c r="E95" s="10"/>
       <c r="F95" s="11"/>
-      <c r="G95" s="18" t="str">
+      <c r="G95" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H95" s="8" t="str">
-        <f>IF(ISBLANK(B95),"--",ROUND(P95*INDEX(Lists!$F$2:$H$5,MATCH(B95,Lists!$F$2:$F$5,0),MATCH(C95,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B95),"--",ROUND(P95*INDEX(Lists!$G$3:$G$5,MATCH(B95,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I95" s="7" t="str">
-        <f>IF($C95="eSurvey+SMS",ROUND(Q95*INDEX(Lists!$F$2:$H$5,MATCH(B95,Lists!$F$2:$F$5,0),MATCH(C95,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C95="eSurvey+SMS",ROUND(Q95*INDEX(Lists!$H$3:$H$5,MATCH(B95,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J95" s="8" t="str">
@@ -6062,16 +6062,16 @@
       <c r="D96" s="12"/>
       <c r="E96" s="10"/>
       <c r="F96" s="11"/>
-      <c r="G96" s="18" t="str">
+      <c r="G96" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H96" s="8" t="str">
-        <f>IF(ISBLANK(B96),"--",ROUND(P96*INDEX(Lists!$F$2:$H$5,MATCH(B96,Lists!$F$2:$F$5,0),MATCH(C96,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B96),"--",ROUND(P96*INDEX(Lists!$G$3:$G$5,MATCH(B96,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I96" s="7" t="str">
-        <f>IF($C96="eSurvey+SMS",ROUND(Q96*INDEX(Lists!$F$2:$H$5,MATCH(B96,Lists!$F$2:$F$5,0),MATCH(C96,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C96="eSurvey+SMS",ROUND(Q96*INDEX(Lists!$H$3:$H$5,MATCH(B96,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J96" s="8" t="str">
@@ -6119,16 +6119,16 @@
       <c r="D97" s="12"/>
       <c r="E97" s="10"/>
       <c r="F97" s="11"/>
-      <c r="G97" s="18" t="str">
+      <c r="G97" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H97" s="8" t="str">
-        <f>IF(ISBLANK(B97),"--",ROUND(P97*INDEX(Lists!$F$2:$H$5,MATCH(B97,Lists!$F$2:$F$5,0),MATCH(C97,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B97),"--",ROUND(P97*INDEX(Lists!$G$3:$G$5,MATCH(B97,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I97" s="7" t="str">
-        <f>IF($C97="eSurvey+SMS",ROUND(Q97*INDEX(Lists!$F$2:$H$5,MATCH(B97,Lists!$F$2:$F$5,0),MATCH(C97,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C97="eSurvey+SMS",ROUND(Q97*INDEX(Lists!$H$3:$H$5,MATCH(B97,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J97" s="8" t="str">
@@ -6176,16 +6176,16 @@
       <c r="D98" s="12"/>
       <c r="E98" s="10"/>
       <c r="F98" s="11"/>
-      <c r="G98" s="18" t="str">
+      <c r="G98" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H98" s="8" t="str">
-        <f>IF(ISBLANK(B98),"--",ROUND(P98*INDEX(Lists!$F$2:$H$5,MATCH(B98,Lists!$F$2:$F$5,0),MATCH(C98,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B98),"--",ROUND(P98*INDEX(Lists!$G$3:$G$5,MATCH(B98,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I98" s="7" t="str">
-        <f>IF($C98="eSurvey+SMS",ROUND(Q98*INDEX(Lists!$F$2:$H$5,MATCH(B98,Lists!$F$2:$F$5,0),MATCH(C98,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C98="eSurvey+SMS",ROUND(Q98*INDEX(Lists!$H$3:$H$5,MATCH(B98,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J98" s="8" t="str">
@@ -6233,16 +6233,16 @@
       <c r="D99" s="12"/>
       <c r="E99" s="10"/>
       <c r="F99" s="11"/>
-      <c r="G99" s="18" t="str">
+      <c r="G99" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H99" s="8" t="str">
-        <f>IF(ISBLANK(B99),"--",ROUND(P99*INDEX(Lists!$F$2:$H$5,MATCH(B99,Lists!$F$2:$F$5,0),MATCH(C99,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B99),"--",ROUND(P99*INDEX(Lists!$G$3:$G$5,MATCH(B99,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I99" s="7" t="str">
-        <f>IF($C99="eSurvey+SMS",ROUND(Q99*INDEX(Lists!$F$2:$H$5,MATCH(B99,Lists!$F$2:$F$5,0),MATCH(C99,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C99="eSurvey+SMS",ROUND(Q99*INDEX(Lists!$H$3:$H$5,MATCH(B99,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J99" s="8" t="str">
@@ -6290,16 +6290,16 @@
       <c r="D100" s="12"/>
       <c r="E100" s="10"/>
       <c r="F100" s="11"/>
-      <c r="G100" s="18" t="str">
+      <c r="G100" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H100" s="8" t="str">
-        <f>IF(ISBLANK(B100),"--",ROUND(P100*INDEX(Lists!$F$2:$H$5,MATCH(B100,Lists!$F$2:$F$5,0),MATCH(C100,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B100),"--",ROUND(P100*INDEX(Lists!$G$3:$G$5,MATCH(B100,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I100" s="7" t="str">
-        <f>IF($C100="eSurvey+SMS",ROUND(Q100*INDEX(Lists!$F$2:$H$5,MATCH(B100,Lists!$F$2:$F$5,0),MATCH(C100,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C100="eSurvey+SMS",ROUND(Q100*INDEX(Lists!$H$3:$H$5,MATCH(B100,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J100" s="8" t="str">
@@ -6347,16 +6347,16 @@
       <c r="D101" s="12"/>
       <c r="E101" s="10"/>
       <c r="F101" s="11"/>
-      <c r="G101" s="18" t="str">
+      <c r="G101" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H101" s="8" t="str">
-        <f>IF(ISBLANK(B101),"--",ROUND(P101*INDEX(Lists!$F$2:$H$5,MATCH(B101,Lists!$F$2:$F$5,0),MATCH(C101,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B101),"--",ROUND(P101*INDEX(Lists!$G$3:$G$5,MATCH(B101,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I101" s="7" t="str">
-        <f>IF($C101="eSurvey+SMS",ROUND(Q101*INDEX(Lists!$F$2:$H$5,MATCH(B101,Lists!$F$2:$F$5,0),MATCH(C101,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C101="eSurvey+SMS",ROUND(Q101*INDEX(Lists!$H$3:$H$5,MATCH(B101,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J101" s="8" t="str">
@@ -6404,16 +6404,16 @@
       <c r="D102" s="12"/>
       <c r="E102" s="10"/>
       <c r="F102" s="11"/>
-      <c r="G102" s="18" t="str">
+      <c r="G102" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H102" s="8" t="str">
-        <f>IF(ISBLANK(B102),"--",ROUND(P102*INDEX(Lists!$F$2:$H$5,MATCH(B102,Lists!$F$2:$F$5,0),MATCH(C102,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B102),"--",ROUND(P102*INDEX(Lists!$G$3:$G$5,MATCH(B102,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I102" s="7" t="str">
-        <f>IF($C102="eSurvey+SMS",ROUND(Q102*INDEX(Lists!$F$2:$H$5,MATCH(B102,Lists!$F$2:$F$5,0),MATCH(C102,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C102="eSurvey+SMS",ROUND(Q102*INDEX(Lists!$H$3:$H$5,MATCH(B102,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J102" s="8" t="str">
@@ -6461,16 +6461,16 @@
       <c r="D103" s="12"/>
       <c r="E103" s="10"/>
       <c r="F103" s="11"/>
-      <c r="G103" s="18" t="str">
+      <c r="G103" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H103" s="8" t="str">
-        <f>IF(ISBLANK(B103),"--",ROUND(P103*INDEX(Lists!$F$2:$H$5,MATCH(B103,Lists!$F$2:$F$5,0),MATCH(C103,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B103),"--",ROUND(P103*INDEX(Lists!$G$3:$G$5,MATCH(B103,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I103" s="7" t="str">
-        <f>IF($C103="eSurvey+SMS",ROUND(Q103*INDEX(Lists!$F$2:$H$5,MATCH(B103,Lists!$F$2:$F$5,0),MATCH(C103,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C103="eSurvey+SMS",ROUND(Q103*INDEX(Lists!$H$3:$H$5,MATCH(B103,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J103" s="8" t="str">
@@ -6518,16 +6518,16 @@
       <c r="D104" s="12"/>
       <c r="E104" s="10"/>
       <c r="F104" s="11"/>
-      <c r="G104" s="18" t="str">
+      <c r="G104" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H104" s="8" t="str">
-        <f>IF(ISBLANK(B104),"--",ROUND(P104*INDEX(Lists!$F$2:$H$5,MATCH(B104,Lists!$F$2:$F$5,0),MATCH(C104,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B104),"--",ROUND(P104*INDEX(Lists!$G$3:$G$5,MATCH(B104,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I104" s="7" t="str">
-        <f>IF($C104="eSurvey+SMS",ROUND(Q104*INDEX(Lists!$F$2:$H$5,MATCH(B104,Lists!$F$2:$F$5,0),MATCH(C104,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C104="eSurvey+SMS",ROUND(Q104*INDEX(Lists!$H$3:$H$5,MATCH(B104,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J104" s="8" t="str">
@@ -6575,16 +6575,16 @@
       <c r="D105" s="12"/>
       <c r="E105" s="10"/>
       <c r="F105" s="11"/>
-      <c r="G105" s="18" t="str">
+      <c r="G105" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H105" s="8" t="str">
-        <f>IF(ISBLANK(B105),"--",ROUND(P105*INDEX(Lists!$F$2:$H$5,MATCH(B105,Lists!$F$2:$F$5,0),MATCH(C105,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B105),"--",ROUND(P105*INDEX(Lists!$G$3:$G$5,MATCH(B105,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I105" s="7" t="str">
-        <f>IF($C105="eSurvey+SMS",ROUND(Q105*INDEX(Lists!$F$2:$H$5,MATCH(B105,Lists!$F$2:$F$5,0),MATCH(C105,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C105="eSurvey+SMS",ROUND(Q105*INDEX(Lists!$H$3:$H$5,MATCH(B105,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J105" s="8" t="str">
@@ -6632,16 +6632,16 @@
       <c r="D106" s="12"/>
       <c r="E106" s="10"/>
       <c r="F106" s="11"/>
-      <c r="G106" s="18" t="str">
+      <c r="G106" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H106" s="8" t="str">
-        <f>IF(ISBLANK(B106),"--",ROUND(P106*INDEX(Lists!$F$2:$H$5,MATCH(B106,Lists!$F$2:$F$5,0),MATCH(C106,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B106),"--",ROUND(P106*INDEX(Lists!$G$3:$G$5,MATCH(B106,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I106" s="7" t="str">
-        <f>IF($C106="eSurvey+SMS",ROUND(Q106*INDEX(Lists!$F$2:$H$5,MATCH(B106,Lists!$F$2:$F$5,0),MATCH(C106,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C106="eSurvey+SMS",ROUND(Q106*INDEX(Lists!$H$3:$H$5,MATCH(B106,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J106" s="8" t="str">
@@ -6689,16 +6689,16 @@
       <c r="D107" s="12"/>
       <c r="E107" s="10"/>
       <c r="F107" s="11"/>
-      <c r="G107" s="18" t="str">
+      <c r="G107" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H107" s="8" t="str">
-        <f>IF(ISBLANK(B107),"--",ROUND(P107*INDEX(Lists!$F$2:$H$5,MATCH(B107,Lists!$F$2:$F$5,0),MATCH(C107,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B107),"--",ROUND(P107*INDEX(Lists!$G$3:$G$5,MATCH(B107,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I107" s="7" t="str">
-        <f>IF($C107="eSurvey+SMS",ROUND(Q107*INDEX(Lists!$F$2:$H$5,MATCH(B107,Lists!$F$2:$F$5,0),MATCH(C107,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C107="eSurvey+SMS",ROUND(Q107*INDEX(Lists!$H$3:$H$5,MATCH(B107,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J107" s="8" t="str">
@@ -6746,16 +6746,16 @@
       <c r="D108" s="12"/>
       <c r="E108" s="10"/>
       <c r="F108" s="11"/>
-      <c r="G108" s="18" t="str">
+      <c r="G108" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H108" s="8" t="str">
-        <f>IF(ISBLANK(B108),"--",ROUND(P108*INDEX(Lists!$F$2:$H$5,MATCH(B108,Lists!$F$2:$F$5,0),MATCH(C108,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B108),"--",ROUND(P108*INDEX(Lists!$G$3:$G$5,MATCH(B108,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I108" s="7" t="str">
-        <f>IF($C108="eSurvey+SMS",ROUND(Q108*INDEX(Lists!$F$2:$H$5,MATCH(B108,Lists!$F$2:$F$5,0),MATCH(C108,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C108="eSurvey+SMS",ROUND(Q108*INDEX(Lists!$H$3:$H$5,MATCH(B108,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J108" s="8" t="str">
@@ -6803,16 +6803,16 @@
       <c r="D109" s="12"/>
       <c r="E109" s="10"/>
       <c r="F109" s="11"/>
-      <c r="G109" s="18" t="str">
+      <c r="G109" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H109" s="8" t="str">
-        <f>IF(ISBLANK(B109),"--",ROUND(P109*INDEX(Lists!$F$2:$H$5,MATCH(B109,Lists!$F$2:$F$5,0),MATCH(C109,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B109),"--",ROUND(P109*INDEX(Lists!$G$3:$G$5,MATCH(B109,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I109" s="7" t="str">
-        <f>IF($C109="eSurvey+SMS",ROUND(Q109*INDEX(Lists!$F$2:$H$5,MATCH(B109,Lists!$F$2:$F$5,0),MATCH(C109,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C109="eSurvey+SMS",ROUND(Q109*INDEX(Lists!$H$3:$H$5,MATCH(B109,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J109" s="8" t="str">
@@ -6860,16 +6860,16 @@
       <c r="D110" s="12"/>
       <c r="E110" s="10"/>
       <c r="F110" s="11"/>
-      <c r="G110" s="18" t="str">
+      <c r="G110" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H110" s="8" t="str">
-        <f>IF(ISBLANK(B110),"--",ROUND(P110*INDEX(Lists!$F$2:$H$5,MATCH(B110,Lists!$F$2:$F$5,0),MATCH(C110,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B110),"--",ROUND(P110*INDEX(Lists!$G$3:$G$5,MATCH(B110,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I110" s="7" t="str">
-        <f>IF($C110="eSurvey+SMS",ROUND(Q110*INDEX(Lists!$F$2:$H$5,MATCH(B110,Lists!$F$2:$F$5,0),MATCH(C110,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C110="eSurvey+SMS",ROUND(Q110*INDEX(Lists!$H$3:$H$5,MATCH(B110,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J110" s="8" t="str">
@@ -6917,16 +6917,16 @@
       <c r="D111" s="12"/>
       <c r="E111" s="10"/>
       <c r="F111" s="11"/>
-      <c r="G111" s="18" t="str">
+      <c r="G111" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H111" s="8" t="str">
-        <f>IF(ISBLANK(B111),"--",ROUND(P111*INDEX(Lists!$F$2:$H$5,MATCH(B111,Lists!$F$2:$F$5,0),MATCH(C111,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B111),"--",ROUND(P111*INDEX(Lists!$G$3:$G$5,MATCH(B111,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I111" s="7" t="str">
-        <f>IF($C111="eSurvey+SMS",ROUND(Q111*INDEX(Lists!$F$2:$H$5,MATCH(B111,Lists!$F$2:$F$5,0),MATCH(C111,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C111="eSurvey+SMS",ROUND(Q111*INDEX(Lists!$H$3:$H$5,MATCH(B111,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J111" s="8" t="str">
@@ -6974,16 +6974,16 @@
       <c r="D112" s="12"/>
       <c r="E112" s="10"/>
       <c r="F112" s="11"/>
-      <c r="G112" s="18" t="str">
+      <c r="G112" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H112" s="8" t="str">
-        <f>IF(ISBLANK(B112),"--",ROUND(P112*INDEX(Lists!$F$2:$H$5,MATCH(B112,Lists!$F$2:$F$5,0),MATCH(C112,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B112),"--",ROUND(P112*INDEX(Lists!$G$3:$G$5,MATCH(B112,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I112" s="7" t="str">
-        <f>IF($C112="eSurvey+SMS",ROUND(Q112*INDEX(Lists!$F$2:$H$5,MATCH(B112,Lists!$F$2:$F$5,0),MATCH(C112,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C112="eSurvey+SMS",ROUND(Q112*INDEX(Lists!$H$3:$H$5,MATCH(B112,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J112" s="8" t="str">
@@ -7031,16 +7031,16 @@
       <c r="D113" s="12"/>
       <c r="E113" s="10"/>
       <c r="F113" s="11"/>
-      <c r="G113" s="18" t="str">
+      <c r="G113" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H113" s="8" t="str">
-        <f>IF(ISBLANK(B113),"--",ROUND(P113*INDEX(Lists!$F$2:$H$5,MATCH(B113,Lists!$F$2:$F$5,0),MATCH(C113,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B113),"--",ROUND(P113*INDEX(Lists!$G$3:$G$5,MATCH(B113,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I113" s="7" t="str">
-        <f>IF($C113="eSurvey+SMS",ROUND(Q113*INDEX(Lists!$F$2:$H$5,MATCH(B113,Lists!$F$2:$F$5,0),MATCH(C113,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C113="eSurvey+SMS",ROUND(Q113*INDEX(Lists!$H$3:$H$5,MATCH(B113,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J113" s="8" t="str">
@@ -7088,16 +7088,16 @@
       <c r="D114" s="12"/>
       <c r="E114" s="10"/>
       <c r="F114" s="11"/>
-      <c r="G114" s="18" t="str">
+      <c r="G114" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H114" s="8" t="str">
-        <f>IF(ISBLANK(B114),"--",ROUND(P114*INDEX(Lists!$F$2:$H$5,MATCH(B114,Lists!$F$2:$F$5,0),MATCH(C114,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B114),"--",ROUND(P114*INDEX(Lists!$G$3:$G$5,MATCH(B114,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I114" s="7" t="str">
-        <f>IF($C114="eSurvey+SMS",ROUND(Q114*INDEX(Lists!$F$2:$H$5,MATCH(B114,Lists!$F$2:$F$5,0),MATCH(C114,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C114="eSurvey+SMS",ROUND(Q114*INDEX(Lists!$H$3:$H$5,MATCH(B114,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J114" s="8" t="str">
@@ -7145,16 +7145,16 @@
       <c r="D115" s="12"/>
       <c r="E115" s="10"/>
       <c r="F115" s="11"/>
-      <c r="G115" s="18" t="str">
+      <c r="G115" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H115" s="8" t="str">
-        <f>IF(ISBLANK(B115),"--",ROUND(P115*INDEX(Lists!$F$2:$H$5,MATCH(B115,Lists!$F$2:$F$5,0),MATCH(C115,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B115),"--",ROUND(P115*INDEX(Lists!$G$3:$G$5,MATCH(B115,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I115" s="7" t="str">
-        <f>IF($C115="eSurvey+SMS",ROUND(Q115*INDEX(Lists!$F$2:$H$5,MATCH(B115,Lists!$F$2:$F$5,0),MATCH(C115,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C115="eSurvey+SMS",ROUND(Q115*INDEX(Lists!$H$3:$H$5,MATCH(B115,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J115" s="8" t="str">
@@ -7202,16 +7202,16 @@
       <c r="D116" s="12"/>
       <c r="E116" s="10"/>
       <c r="F116" s="11"/>
-      <c r="G116" s="18" t="str">
+      <c r="G116" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H116" s="8" t="str">
-        <f>IF(ISBLANK(B116),"--",ROUND(P116*INDEX(Lists!$F$2:$H$5,MATCH(B116,Lists!$F$2:$F$5,0),MATCH(C116,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B116),"--",ROUND(P116*INDEX(Lists!$G$3:$G$5,MATCH(B116,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I116" s="7" t="str">
-        <f>IF($C116="eSurvey+SMS",ROUND(Q116*INDEX(Lists!$F$2:$H$5,MATCH(B116,Lists!$F$2:$F$5,0),MATCH(C116,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C116="eSurvey+SMS",ROUND(Q116*INDEX(Lists!$H$3:$H$5,MATCH(B116,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J116" s="8" t="str">
@@ -7259,16 +7259,16 @@
       <c r="D117" s="12"/>
       <c r="E117" s="10"/>
       <c r="F117" s="11"/>
-      <c r="G117" s="18" t="str">
+      <c r="G117" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H117" s="8" t="str">
-        <f>IF(ISBLANK(B117),"--",ROUND(P117*INDEX(Lists!$F$2:$H$5,MATCH(B117,Lists!$F$2:$F$5,0),MATCH(C117,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B117),"--",ROUND(P117*INDEX(Lists!$G$3:$G$5,MATCH(B117,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I117" s="7" t="str">
-        <f>IF($C117="eSurvey+SMS",ROUND(Q117*INDEX(Lists!$F$2:$H$5,MATCH(B117,Lists!$F$2:$F$5,0),MATCH(C117,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C117="eSurvey+SMS",ROUND(Q117*INDEX(Lists!$H$3:$H$5,MATCH(B117,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J117" s="8" t="str">
@@ -7316,16 +7316,16 @@
       <c r="D118" s="12"/>
       <c r="E118" s="10"/>
       <c r="F118" s="11"/>
-      <c r="G118" s="18" t="str">
+      <c r="G118" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H118" s="8" t="str">
-        <f>IF(ISBLANK(B118),"--",ROUND(P118*INDEX(Lists!$F$2:$H$5,MATCH(B118,Lists!$F$2:$F$5,0),MATCH(C118,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B118),"--",ROUND(P118*INDEX(Lists!$G$3:$G$5,MATCH(B118,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I118" s="7" t="str">
-        <f>IF($C118="eSurvey+SMS",ROUND(Q118*INDEX(Lists!$F$2:$H$5,MATCH(B118,Lists!$F$2:$F$5,0),MATCH(C118,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C118="eSurvey+SMS",ROUND(Q118*INDEX(Lists!$H$3:$H$5,MATCH(B118,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J118" s="8" t="str">
@@ -7373,16 +7373,16 @@
       <c r="D119" s="12"/>
       <c r="E119" s="10"/>
       <c r="F119" s="11"/>
-      <c r="G119" s="18" t="str">
+      <c r="G119" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H119" s="8" t="str">
-        <f>IF(ISBLANK(B119),"--",ROUND(P119*INDEX(Lists!$F$2:$H$5,MATCH(B119,Lists!$F$2:$F$5,0),MATCH(C119,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B119),"--",ROUND(P119*INDEX(Lists!$G$3:$G$5,MATCH(B119,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I119" s="7" t="str">
-        <f>IF($C119="eSurvey+SMS",ROUND(Q119*INDEX(Lists!$F$2:$H$5,MATCH(B119,Lists!$F$2:$F$5,0),MATCH(C119,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C119="eSurvey+SMS",ROUND(Q119*INDEX(Lists!$H$3:$H$5,MATCH(B119,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J119" s="8" t="str">
@@ -7430,16 +7430,16 @@
       <c r="D120" s="12"/>
       <c r="E120" s="10"/>
       <c r="F120" s="11"/>
-      <c r="G120" s="18" t="str">
+      <c r="G120" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H120" s="8" t="str">
-        <f>IF(ISBLANK(B120),"--",ROUND(P120*INDEX(Lists!$F$2:$H$5,MATCH(B120,Lists!$F$2:$F$5,0),MATCH(C120,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B120),"--",ROUND(P120*INDEX(Lists!$G$3:$G$5,MATCH(B120,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I120" s="7" t="str">
-        <f>IF($C120="eSurvey+SMS",ROUND(Q120*INDEX(Lists!$F$2:$H$5,MATCH(B120,Lists!$F$2:$F$5,0),MATCH(C120,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C120="eSurvey+SMS",ROUND(Q120*INDEX(Lists!$H$3:$H$5,MATCH(B120,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J120" s="8" t="str">
@@ -7487,16 +7487,16 @@
       <c r="D121" s="12"/>
       <c r="E121" s="10"/>
       <c r="F121" s="11"/>
-      <c r="G121" s="18" t="str">
+      <c r="G121" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H121" s="8" t="str">
-        <f>IF(ISBLANK(B121),"--",ROUND(P121*INDEX(Lists!$F$2:$H$5,MATCH(B121,Lists!$F$2:$F$5,0),MATCH(C121,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B121),"--",ROUND(P121*INDEX(Lists!$G$3:$G$5,MATCH(B121,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I121" s="7" t="str">
-        <f>IF($C121="eSurvey+SMS",ROUND(Q121*INDEX(Lists!$F$2:$H$5,MATCH(B121,Lists!$F$2:$F$5,0),MATCH(C121,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C121="eSurvey+SMS",ROUND(Q121*INDEX(Lists!$H$3:$H$5,MATCH(B121,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J121" s="8" t="str">
@@ -7544,16 +7544,16 @@
       <c r="D122" s="12"/>
       <c r="E122" s="10"/>
       <c r="F122" s="11"/>
-      <c r="G122" s="18" t="str">
+      <c r="G122" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H122" s="8" t="str">
-        <f>IF(ISBLANK(B122),"--",ROUND(P122*INDEX(Lists!$F$2:$H$5,MATCH(B122,Lists!$F$2:$F$5,0),MATCH(C122,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B122),"--",ROUND(P122*INDEX(Lists!$G$3:$G$5,MATCH(B122,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I122" s="7" t="str">
-        <f>IF($C122="eSurvey+SMS",ROUND(Q122*INDEX(Lists!$F$2:$H$5,MATCH(B122,Lists!$F$2:$F$5,0),MATCH(C122,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C122="eSurvey+SMS",ROUND(Q122*INDEX(Lists!$H$3:$H$5,MATCH(B122,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J122" s="8" t="str">
@@ -7601,16 +7601,16 @@
       <c r="D123" s="12"/>
       <c r="E123" s="10"/>
       <c r="F123" s="11"/>
-      <c r="G123" s="18" t="str">
+      <c r="G123" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H123" s="8" t="str">
-        <f>IF(ISBLANK(B123),"--",ROUND(P123*INDEX(Lists!$F$2:$H$5,MATCH(B123,Lists!$F$2:$F$5,0),MATCH(C123,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B123),"--",ROUND(P123*INDEX(Lists!$G$3:$G$5,MATCH(B123,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I123" s="7" t="str">
-        <f>IF($C123="eSurvey+SMS",ROUND(Q123*INDEX(Lists!$F$2:$H$5,MATCH(B123,Lists!$F$2:$F$5,0),MATCH(C123,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C123="eSurvey+SMS",ROUND(Q123*INDEX(Lists!$H$3:$H$5,MATCH(B123,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J123" s="8" t="str">
@@ -7658,16 +7658,16 @@
       <c r="D124" s="12"/>
       <c r="E124" s="10"/>
       <c r="F124" s="11"/>
-      <c r="G124" s="18" t="str">
+      <c r="G124" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H124" s="8" t="str">
-        <f>IF(ISBLANK(B124),"--",ROUND(P124*INDEX(Lists!$F$2:$H$5,MATCH(B124,Lists!$F$2:$F$5,0),MATCH(C124,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B124),"--",ROUND(P124*INDEX(Lists!$G$3:$G$5,MATCH(B124,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I124" s="7" t="str">
-        <f>IF($C124="eSurvey+SMS",ROUND(Q124*INDEX(Lists!$F$2:$H$5,MATCH(B124,Lists!$F$2:$F$5,0),MATCH(C124,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C124="eSurvey+SMS",ROUND(Q124*INDEX(Lists!$H$3:$H$5,MATCH(B124,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J124" s="8" t="str">
@@ -7715,16 +7715,16 @@
       <c r="D125" s="12"/>
       <c r="E125" s="10"/>
       <c r="F125" s="11"/>
-      <c r="G125" s="18" t="str">
+      <c r="G125" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H125" s="8" t="str">
-        <f>IF(ISBLANK(B125),"--",ROUND(P125*INDEX(Lists!$F$2:$H$5,MATCH(B125,Lists!$F$2:$F$5,0),MATCH(C125,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B125),"--",ROUND(P125*INDEX(Lists!$G$3:$G$5,MATCH(B125,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I125" s="7" t="str">
-        <f>IF($C125="eSurvey+SMS",ROUND(Q125*INDEX(Lists!$F$2:$H$5,MATCH(B125,Lists!$F$2:$F$5,0),MATCH(C125,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C125="eSurvey+SMS",ROUND(Q125*INDEX(Lists!$H$3:$H$5,MATCH(B125,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J125" s="8" t="str">
@@ -7772,16 +7772,16 @@
       <c r="D126" s="12"/>
       <c r="E126" s="10"/>
       <c r="F126" s="11"/>
-      <c r="G126" s="18" t="str">
+      <c r="G126" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H126" s="8" t="str">
-        <f>IF(ISBLANK(B126),"--",ROUND(P126*INDEX(Lists!$F$2:$H$5,MATCH(B126,Lists!$F$2:$F$5,0),MATCH(C126,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B126),"--",ROUND(P126*INDEX(Lists!$G$3:$G$5,MATCH(B126,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I126" s="7" t="str">
-        <f>IF($C126="eSurvey+SMS",ROUND(Q126*INDEX(Lists!$F$2:$H$5,MATCH(B126,Lists!$F$2:$F$5,0),MATCH(C126,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C126="eSurvey+SMS",ROUND(Q126*INDEX(Lists!$H$3:$H$5,MATCH(B126,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J126" s="8" t="str">
@@ -7829,16 +7829,16 @@
       <c r="D127" s="12"/>
       <c r="E127" s="10"/>
       <c r="F127" s="11"/>
-      <c r="G127" s="18" t="str">
+      <c r="G127" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H127" s="8" t="str">
-        <f>IF(ISBLANK(B127),"--",ROUND(P127*INDEX(Lists!$F$2:$H$5,MATCH(B127,Lists!$F$2:$F$5,0),MATCH(C127,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B127),"--",ROUND(P127*INDEX(Lists!$G$3:$G$5,MATCH(B127,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I127" s="7" t="str">
-        <f>IF($C127="eSurvey+SMS",ROUND(Q127*INDEX(Lists!$F$2:$H$5,MATCH(B127,Lists!$F$2:$F$5,0),MATCH(C127,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C127="eSurvey+SMS",ROUND(Q127*INDEX(Lists!$H$3:$H$5,MATCH(B127,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J127" s="8" t="str">
@@ -7886,16 +7886,16 @@
       <c r="D128" s="12"/>
       <c r="E128" s="10"/>
       <c r="F128" s="11"/>
-      <c r="G128" s="18" t="str">
+      <c r="G128" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H128" s="8" t="str">
-        <f>IF(ISBLANK(B128),"--",ROUND(P128*INDEX(Lists!$F$2:$H$5,MATCH(B128,Lists!$F$2:$F$5,0),MATCH(C128,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B128),"--",ROUND(P128*INDEX(Lists!$G$3:$G$5,MATCH(B128,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I128" s="7" t="str">
-        <f>IF($C128="eSurvey+SMS",ROUND(Q128*INDEX(Lists!$F$2:$H$5,MATCH(B128,Lists!$F$2:$F$5,0),MATCH(C128,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C128="eSurvey+SMS",ROUND(Q128*INDEX(Lists!$H$3:$H$5,MATCH(B128,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J128" s="8" t="str">
@@ -7943,16 +7943,16 @@
       <c r="D129" s="12"/>
       <c r="E129" s="10"/>
       <c r="F129" s="11"/>
-      <c r="G129" s="18" t="str">
+      <c r="G129" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H129" s="8" t="str">
-        <f>IF(ISBLANK(B129),"--",ROUND(P129*INDEX(Lists!$F$2:$H$5,MATCH(B129,Lists!$F$2:$F$5,0),MATCH(C129,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B129),"--",ROUND(P129*INDEX(Lists!$G$3:$G$5,MATCH(B129,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I129" s="7" t="str">
-        <f>IF($C129="eSurvey+SMS",ROUND(Q129*INDEX(Lists!$F$2:$H$5,MATCH(B129,Lists!$F$2:$F$5,0),MATCH(C129,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C129="eSurvey+SMS",ROUND(Q129*INDEX(Lists!$H$3:$H$5,MATCH(B129,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J129" s="8" t="str">
@@ -8000,16 +8000,16 @@
       <c r="D130" s="12"/>
       <c r="E130" s="10"/>
       <c r="F130" s="11"/>
-      <c r="G130" s="18" t="str">
+      <c r="G130" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H130" s="8" t="str">
-        <f>IF(ISBLANK(B130),"--",ROUND(P130*INDEX(Lists!$F$2:$H$5,MATCH(B130,Lists!$F$2:$F$5,0),MATCH(C130,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B130),"--",ROUND(P130*INDEX(Lists!$G$3:$G$5,MATCH(B130,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I130" s="7" t="str">
-        <f>IF($C130="eSurvey+SMS",ROUND(Q130*INDEX(Lists!$F$2:$H$5,MATCH(B130,Lists!$F$2:$F$5,0),MATCH(C130,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C130="eSurvey+SMS",ROUND(Q130*INDEX(Lists!$H$3:$H$5,MATCH(B130,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J130" s="8" t="str">
@@ -8057,16 +8057,16 @@
       <c r="D131" s="12"/>
       <c r="E131" s="10"/>
       <c r="F131" s="11"/>
-      <c r="G131" s="18" t="str">
+      <c r="G131" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H131" s="8" t="str">
-        <f>IF(ISBLANK(B131),"--",ROUND(P131*INDEX(Lists!$F$2:$H$5,MATCH(B131,Lists!$F$2:$F$5,0),MATCH(C131,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B131),"--",ROUND(P131*INDEX(Lists!$G$3:$G$5,MATCH(B131,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I131" s="7" t="str">
-        <f>IF($C131="eSurvey+SMS",ROUND(Q131*INDEX(Lists!$F$2:$H$5,MATCH(B131,Lists!$F$2:$F$5,0),MATCH(C131,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C131="eSurvey+SMS",ROUND(Q131*INDEX(Lists!$H$3:$H$5,MATCH(B131,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J131" s="8" t="str">
@@ -8114,16 +8114,16 @@
       <c r="D132" s="12"/>
       <c r="E132" s="10"/>
       <c r="F132" s="11"/>
-      <c r="G132" s="18" t="str">
+      <c r="G132" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H132" s="8" t="str">
-        <f>IF(ISBLANK(B132),"--",ROUND(P132*INDEX(Lists!$F$2:$H$5,MATCH(B132,Lists!$F$2:$F$5,0),MATCH(C132,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B132),"--",ROUND(P132*INDEX(Lists!$G$3:$G$5,MATCH(B132,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I132" s="7" t="str">
-        <f>IF($C132="eSurvey+SMS",ROUND(Q132*INDEX(Lists!$F$2:$H$5,MATCH(B132,Lists!$F$2:$F$5,0),MATCH(C132,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C132="eSurvey+SMS",ROUND(Q132*INDEX(Lists!$H$3:$H$5,MATCH(B132,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J132" s="8" t="str">
@@ -8171,16 +8171,16 @@
       <c r="D133" s="12"/>
       <c r="E133" s="10"/>
       <c r="F133" s="11"/>
-      <c r="G133" s="18" t="str">
+      <c r="G133" s="16" t="str">
         <f t="shared" si="8"/>
         <v>--</v>
       </c>
       <c r="H133" s="8" t="str">
-        <f>IF(ISBLANK(B133),"--",ROUND(P133*INDEX(Lists!$F$2:$H$5,MATCH(B133,Lists!$F$2:$F$5,0),MATCH(C133,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B133),"--",ROUND(P133*INDEX(Lists!$G$3:$G$5,MATCH(B133,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I133" s="7" t="str">
-        <f>IF($C133="eSurvey+SMS",ROUND(Q133*INDEX(Lists!$F$2:$H$5,MATCH(B133,Lists!$F$2:$F$5,0),MATCH(C133,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C133="eSurvey+SMS",ROUND(Q133*INDEX(Lists!$H$3:$H$5,MATCH(B133,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J133" s="8" t="str">
@@ -8228,16 +8228,16 @@
       <c r="D134" s="12"/>
       <c r="E134" s="10"/>
       <c r="F134" s="11"/>
-      <c r="G134" s="18" t="str">
+      <c r="G134" s="16" t="str">
         <f t="shared" ref="G134:G138" si="16">IF(ISBLANK(B134),"--",SUM(H134,I134))</f>
         <v>--</v>
       </c>
       <c r="H134" s="8" t="str">
-        <f>IF(ISBLANK(B134),"--",ROUND(P134*INDEX(Lists!$F$2:$H$5,MATCH(B134,Lists!$F$2:$F$5,0),MATCH(C134,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B134),"--",ROUND(P134*INDEX(Lists!$G$3:$G$5,MATCH(B134,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I134" s="7" t="str">
-        <f>IF($C134="eSurvey+SMS",ROUND(Q134*INDEX(Lists!$F$2:$H$5,MATCH(B134,Lists!$F$2:$F$5,0),MATCH(C134,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C134="eSurvey+SMS",ROUND(Q134*INDEX(Lists!$H$3:$H$5,MATCH(B134,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J134" s="8" t="str">
@@ -8285,16 +8285,16 @@
       <c r="D135" s="12"/>
       <c r="E135" s="10"/>
       <c r="F135" s="11"/>
-      <c r="G135" s="18" t="str">
+      <c r="G135" s="16" t="str">
         <f t="shared" si="16"/>
         <v>--</v>
       </c>
       <c r="H135" s="8" t="str">
-        <f>IF(ISBLANK(B135),"--",ROUND(P135*INDEX(Lists!$F$2:$H$5,MATCH(B135,Lists!$F$2:$F$5,0),MATCH(C135,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B135),"--",ROUND(P135*INDEX(Lists!$G$3:$G$5,MATCH(B135,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I135" s="7" t="str">
-        <f>IF($C135="eSurvey+SMS",ROUND(Q135*INDEX(Lists!$F$2:$H$5,MATCH(B135,Lists!$F$2:$F$5,0),MATCH(C135,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C135="eSurvey+SMS",ROUND(Q135*INDEX(Lists!$H$3:$H$5,MATCH(B135,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J135" s="8" t="str">
@@ -8342,16 +8342,16 @@
       <c r="D136" s="12"/>
       <c r="E136" s="10"/>
       <c r="F136" s="11"/>
-      <c r="G136" s="18" t="str">
+      <c r="G136" s="16" t="str">
         <f t="shared" si="16"/>
         <v>--</v>
       </c>
       <c r="H136" s="8" t="str">
-        <f>IF(ISBLANK(B136),"--",ROUND(P136*INDEX(Lists!$F$2:$H$5,MATCH(B136,Lists!$F$2:$F$5,0),MATCH(C136,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B136),"--",ROUND(P136*INDEX(Lists!$G$3:$G$5,MATCH(B136,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I136" s="7" t="str">
-        <f>IF($C136="eSurvey+SMS",ROUND(Q136*INDEX(Lists!$F$2:$H$5,MATCH(B136,Lists!$F$2:$F$5,0),MATCH(C136,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C136="eSurvey+SMS",ROUND(Q136*INDEX(Lists!$H$3:$H$5,MATCH(B136,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J136" s="8" t="str">
@@ -8399,16 +8399,16 @@
       <c r="D137" s="12"/>
       <c r="E137" s="10"/>
       <c r="F137" s="11"/>
-      <c r="G137" s="18" t="str">
+      <c r="G137" s="16" t="str">
         <f t="shared" si="16"/>
         <v>--</v>
       </c>
       <c r="H137" s="8" t="str">
-        <f>IF(ISBLANK(B137),"--",ROUND(P137*INDEX(Lists!$F$2:$H$5,MATCH(B137,Lists!$F$2:$F$5,0),MATCH(C137,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B137),"--",ROUND(P137*INDEX(Lists!$G$3:$G$5,MATCH(B137,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I137" s="7" t="str">
-        <f>IF($C137="eSurvey+SMS",ROUND(Q137*INDEX(Lists!$F$2:$H$5,MATCH(B137,Lists!$F$2:$F$5,0),MATCH(C137,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C137="eSurvey+SMS",ROUND(Q137*INDEX(Lists!$H$3:$H$5,MATCH(B137,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J137" s="8" t="str">
@@ -8456,16 +8456,16 @@
       <c r="D138" s="12"/>
       <c r="E138" s="10"/>
       <c r="F138" s="11"/>
-      <c r="G138" s="18" t="str">
+      <c r="G138" s="16" t="str">
         <f t="shared" si="16"/>
         <v>--</v>
       </c>
       <c r="H138" s="8" t="str">
-        <f>IF(ISBLANK(B138),"--",ROUND(P138*INDEX(Lists!$F$2:$H$5,MATCH(B138,Lists!$F$2:$F$5,0),MATCH(C138,Lists!$F$2:$H$2,0)),0))</f>
+        <f>IF(ISBLANK(B138),"--",ROUND(P138*INDEX(Lists!$G$3:$G$5,MATCH(B138,Lists!$F$3:$F$5,0)),0))</f>
         <v>--</v>
       </c>
       <c r="I138" s="7" t="str">
-        <f>IF($C138="eSurvey+SMS",ROUND(Q138*INDEX(Lists!$F$2:$H$5,MATCH(B138,Lists!$F$2:$F$5,0),MATCH(C138,Lists!$F$2:$H$2,0)),0),"--")</f>
+        <f>IF($C138="eSurvey+SMS",ROUND(Q138*INDEX(Lists!$H$3:$H$5,MATCH(B138,Lists!$F$3:$F$5,0)),0),"--")</f>
         <v>--</v>
       </c>
       <c r="J138" s="8" t="str">
@@ -8507,21 +8507,21 @@
       <c r="V138" s="1"/>
     </row>
     <row r="139" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A139" s="15" t="s">
+      <c r="A139" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B139" s="15"/>
-      <c r="C139" s="15"/>
-      <c r="D139" s="15"/>
-      <c r="E139" s="15"/>
-      <c r="F139" s="15"/>
-      <c r="G139" s="15"/>
-      <c r="H139" s="15"/>
-      <c r="I139" s="15"/>
-      <c r="J139" s="15"/>
-      <c r="K139" s="15"/>
-      <c r="L139" s="15"/>
-      <c r="M139" s="15"/>
+      <c r="B139" s="19"/>
+      <c r="C139" s="19"/>
+      <c r="D139" s="19"/>
+      <c r="E139" s="19"/>
+      <c r="F139" s="19"/>
+      <c r="G139" s="19"/>
+      <c r="H139" s="19"/>
+      <c r="I139" s="19"/>
+      <c r="J139" s="19"/>
+      <c r="K139" s="19"/>
+      <c r="L139" s="19"/>
+      <c r="M139" s="19"/>
       <c r="N139" s="1"/>
       <c r="O139" s="1"/>
       <c r="P139" s="1"/>
@@ -9573,7 +9573,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9595,16 +9595,16 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="J1" s="16" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="J1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -9646,7 +9646,7 @@
         <v>0.22</v>
       </c>
       <c r="H3" s="13">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="J3" t="s">
         <v>2</v>
@@ -9666,19 +9666,19 @@
         <v>3</v>
       </c>
       <c r="G4" s="13">
-        <v>0.15</v>
+        <v>0.09</v>
       </c>
       <c r="H4" s="13">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="J4" t="s">
         <v>3</v>
       </c>
       <c r="K4" s="13">
-        <v>0.66</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="L4" s="13">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -9686,19 +9686,19 @@
         <v>4</v>
       </c>
       <c r="G5" s="13">
-        <v>7.0000000000000007E-2</v>
+        <v>0.19</v>
       </c>
       <c r="H5" s="13">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
       <c r="J5" t="s">
         <v>4</v>
       </c>
       <c r="K5" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.66</v>
       </c>
       <c r="L5" s="13">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>